<commit_message>
0613 (src udt) 이가원
</commit_message>
<xml_diff>
--- a/docs/요구사항정의서.xlsx
+++ b/docs/요구사항정의서.xlsx
@@ -3747,6 +3747,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3762,6 +3783,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3769,36 +3799,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4092,9 +4092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4140,10 +4140,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -4169,8 +4169,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="2" t="s">
         <v>119</v>
       </c>
@@ -4192,8 +4192,8 @@
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="2" t="s">
         <v>121</v>
       </c>
@@ -4215,8 +4215,8 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="2" t="s">
         <v>122</v>
       </c>
@@ -4238,8 +4238,8 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -4261,8 +4261,8 @@
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="2" t="s">
         <v>132</v>
       </c>
@@ -4284,8 +4284,8 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="2" t="s">
         <v>134</v>
       </c>
@@ -4307,8 +4307,8 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="2" t="s">
         <v>170</v>
       </c>
@@ -4330,8 +4330,8 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="2" t="s">
         <v>301</v>
       </c>
@@ -4353,8 +4353,8 @@
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
@@ -4374,8 +4374,8 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="2" t="s">
         <v>141</v>
       </c>
@@ -4395,8 +4395,8 @@
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="2" t="s">
         <v>144</v>
       </c>
@@ -4416,8 +4416,8 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="2" t="s">
         <v>148</v>
       </c>
@@ -4437,8 +4437,8 @@
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="2" t="s">
         <v>152</v>
       </c>
@@ -4458,8 +4458,8 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="2" t="s">
         <v>160</v>
       </c>
@@ -4479,8 +4479,8 @@
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="2" t="s">
         <v>163</v>
       </c>
@@ -4500,8 +4500,8 @@
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="2" t="s">
         <v>164</v>
       </c>
@@ -4521,10 +4521,10 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -4548,8 +4548,8 @@
       <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
@@ -4569,13 +4569,13 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -4598,9 +4598,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="33"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="4" t="s">
         <v>179</v>
       </c>
@@ -4621,9 +4621,9 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="33"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="4" t="s">
         <v>190</v>
       </c>
@@ -4644,8 +4644,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -4665,8 +4665,8 @@
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
@@ -4686,8 +4686,8 @@
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="4" t="s">
         <v>185</v>
       </c>
@@ -4707,8 +4707,8 @@
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="4" t="s">
         <v>188</v>
       </c>
@@ -4728,8 +4728,8 @@
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="4" t="s">
         <v>195</v>
       </c>
@@ -4749,13 +4749,13 @@
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="33" t="s">
         <v>155</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -4776,9 +4776,9 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="34"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="5" t="s">
         <v>423</v>
       </c>
@@ -4797,8 +4797,8 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="5" t="s">
         <v>156</v>
       </c>
@@ -4818,8 +4818,8 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="5" t="s">
         <v>207</v>
       </c>
@@ -4839,8 +4839,8 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="5" t="s">
         <v>212</v>
       </c>
@@ -4860,8 +4860,8 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="5" t="s">
         <v>157</v>
       </c>
@@ -4881,8 +4881,8 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="5" t="s">
         <v>201</v>
       </c>
@@ -4902,8 +4902,8 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="5" t="s">
         <v>204</v>
       </c>
@@ -4923,10 +4923,10 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -4952,8 +4952,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="6" t="s">
         <v>227</v>
       </c>
@@ -4975,8 +4975,8 @@
       <c r="I38" s="11"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="6" t="s">
         <v>230</v>
       </c>
@@ -4998,8 +4998,8 @@
       <c r="I39" s="11"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="6" t="s">
         <v>22</v>
       </c>
@@ -5019,8 +5019,8 @@
       <c r="I40" s="11"/>
     </row>
     <row r="41" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="6" t="s">
         <v>220</v>
       </c>
@@ -5040,8 +5040,8 @@
       <c r="I41" s="11"/>
     </row>
     <row r="42" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="21"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="6" t="s">
         <v>223</v>
       </c>
@@ -5061,8 +5061,8 @@
       <c r="I42" s="11"/>
     </row>
     <row r="43" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="6" t="s">
         <v>226</v>
       </c>
@@ -5082,8 +5082,8 @@
       <c r="I43" s="11"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="6" t="s">
         <v>23</v>
       </c>
@@ -5103,10 +5103,10 @@
       <c r="I44" s="11"/>
     </row>
     <row r="45" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="22" t="s">
         <v>29</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -5130,8 +5130,8 @@
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="2" t="s">
         <v>237</v>
       </c>
@@ -5153,8 +5153,8 @@
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="2" t="s">
         <v>243</v>
       </c>
@@ -5176,8 +5176,8 @@
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="2" t="s">
         <v>756</v>
       </c>
@@ -5199,8 +5199,8 @@
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="2" t="s">
         <v>31</v>
       </c>
@@ -5220,8 +5220,8 @@
       <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="2" t="s">
         <v>761</v>
       </c>
@@ -5241,8 +5241,8 @@
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="2" t="s">
         <v>760</v>
       </c>
@@ -5262,10 +5262,10 @@
       <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="23" t="s">
         <v>328</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -5289,8 +5289,8 @@
       <c r="I52" s="8"/>
     </row>
     <row r="53" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="3" t="s">
         <v>773</v>
       </c>
@@ -5312,8 +5312,8 @@
       <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="3" t="s">
         <v>330</v>
       </c>
@@ -5335,8 +5335,8 @@
       <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="3" t="s">
         <v>331</v>
       </c>
@@ -5358,8 +5358,8 @@
       <c r="I55" s="8"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="3" t="s">
         <v>332</v>
       </c>
@@ -5379,8 +5379,8 @@
       <c r="I56" s="8"/>
     </row>
     <row r="57" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="3" t="s">
         <v>333</v>
       </c>
@@ -5402,8 +5402,8 @@
       <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="37"/>
-      <c r="B58" s="37"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="3" t="s">
         <v>334</v>
       </c>
@@ -5423,10 +5423,10 @@
       <c r="I58" s="8"/>
     </row>
     <row r="59" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="29" t="s">
         <v>437</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="29" t="s">
         <v>438</v>
       </c>
       <c r="C59" s="15" t="s">
@@ -5450,8 +5450,8 @@
       <c r="I59" s="14"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="15" t="s">
         <v>494</v>
       </c>
@@ -5471,8 +5471,8 @@
       <c r="I60" s="16"/>
     </row>
     <row r="61" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="15" t="s">
         <v>495</v>
       </c>
@@ -5492,8 +5492,8 @@
       <c r="I61" s="16"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="23"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
       <c r="C62" s="15" t="s">
         <v>446</v>
       </c>
@@ -5513,8 +5513,8 @@
       <c r="I62" s="14"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="23"/>
-      <c r="B63" s="23"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="30"/>
       <c r="C63" s="15" t="s">
         <v>447</v>
       </c>
@@ -5534,8 +5534,8 @@
       <c r="I63" s="14"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="23"/>
-      <c r="B64" s="23"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="30"/>
       <c r="C64" s="15" t="s">
         <v>493</v>
       </c>
@@ -5555,8 +5555,8 @@
       <c r="I64" s="14"/>
     </row>
     <row r="65" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="15" t="s">
         <v>492</v>
       </c>
@@ -5576,10 +5576,10 @@
       <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -5603,8 +5603,8 @@
       <c r="I66" s="9"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="4" t="s">
         <v>35</v>
       </c>
@@ -5624,8 +5624,8 @@
       <c r="I67" s="9"/>
     </row>
     <row r="68" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="26"/>
       <c r="C68" s="4" t="s">
         <v>466</v>
       </c>
@@ -5645,8 +5645,8 @@
       <c r="I68" s="9"/>
     </row>
     <row r="69" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="30"/>
-      <c r="B69" s="30"/>
+      <c r="A69" s="26"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="4" t="s">
         <v>490</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>501</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>733</v>
+        <v>247</v>
       </c>
       <c r="H69" s="9" t="s">
         <v>487</v>
@@ -5668,8 +5668,8 @@
       <c r="I69" s="9"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="30"/>
-      <c r="B70" s="30"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="4" t="s">
         <v>36</v>
       </c>
@@ -5689,8 +5689,8 @@
       <c r="I70" s="9"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="30"/>
-      <c r="B71" s="30"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="26"/>
       <c r="C71" s="4" t="s">
         <v>440</v>
       </c>
@@ -5710,10 +5710,10 @@
       <c r="I71" s="9"/>
     </row>
     <row r="72" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A72" s="20" t="s">
+      <c r="A72" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="27" t="s">
         <v>460</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -5737,8 +5737,8 @@
       <c r="I72" s="10"/>
     </row>
     <row r="73" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
       <c r="C73" s="5" t="s">
         <v>508</v>
       </c>
@@ -5760,8 +5760,8 @@
       <c r="I73" s="10"/>
     </row>
     <row r="74" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="5" t="s">
         <v>509</v>
       </c>
@@ -5783,8 +5783,8 @@
       <c r="I74" s="10"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
       <c r="C75" s="5" t="s">
         <v>512</v>
       </c>
@@ -5804,8 +5804,8 @@
       <c r="I75" s="10"/>
     </row>
     <row r="76" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
       <c r="C76" s="5" t="s">
         <v>463</v>
       </c>
@@ -5825,10 +5825,10 @@
       <c r="I76" s="10"/>
     </row>
     <row r="77" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="21" t="s">
+      <c r="A77" s="28" t="s">
         <v>506</v>
       </c>
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="28" t="s">
         <v>526</v>
       </c>
       <c r="C77" s="6" t="s">
@@ -5852,8 +5852,8 @@
       <c r="I77" s="11"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="21"/>
-      <c r="B78" s="21"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="28"/>
       <c r="C78" s="6" t="s">
         <v>521</v>
       </c>
@@ -5873,8 +5873,8 @@
       <c r="I78" s="11"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="21"/>
-      <c r="B79" s="21"/>
+      <c r="A79" s="28"/>
+      <c r="B79" s="28"/>
       <c r="C79" s="6" t="s">
         <v>532</v>
       </c>
@@ -5894,10 +5894,10 @@
       <c r="I79" s="11"/>
     </row>
     <row r="80" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A80" s="28" t="s">
+      <c r="A80" s="22" t="s">
         <v>522</v>
       </c>
-      <c r="B80" s="28" t="s">
+      <c r="B80" s="22" t="s">
         <v>507</v>
       </c>
       <c r="C80" s="2" t="s">
@@ -5921,8 +5921,8 @@
       <c r="I80" s="7"/>
     </row>
     <row r="81" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
       <c r="C81" s="2" t="s">
         <v>524</v>
       </c>
@@ -5944,8 +5944,8 @@
       <c r="I81" s="7"/>
     </row>
     <row r="82" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="28"/>
-      <c r="B82" s="28"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
       <c r="C82" s="2" t="s">
         <v>538</v>
       </c>
@@ -5967,8 +5967,8 @@
       <c r="I82" s="7"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="28"/>
-      <c r="B83" s="28"/>
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
       <c r="C83" s="2" t="s">
         <v>544</v>
       </c>
@@ -5990,8 +5990,8 @@
       <c r="I83" s="7"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="28"/>
-      <c r="B84" s="28"/>
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
       <c r="C84" s="2" t="s">
         <v>525</v>
       </c>
@@ -6011,10 +6011,10 @@
       <c r="I84" s="7"/>
     </row>
     <row r="85" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B85" s="29" t="s">
+      <c r="B85" s="21" t="s">
         <v>551</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -6038,8 +6038,8 @@
       <c r="I85" s="8"/>
     </row>
     <row r="86" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A86" s="29"/>
-      <c r="B86" s="29"/>
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
       <c r="C86" s="3" t="s">
         <v>558</v>
       </c>
@@ -6059,8 +6059,8 @@
       <c r="I86" s="8"/>
     </row>
     <row r="87" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="29"/>
-      <c r="B87" s="29"/>
+      <c r="A87" s="21"/>
+      <c r="B87" s="21"/>
       <c r="C87" s="3" t="s">
         <v>557</v>
       </c>
@@ -6082,8 +6082,8 @@
       <c r="I87" s="8"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="29"/>
-      <c r="B88" s="29"/>
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
       <c r="C88" s="3" t="s">
         <v>40</v>
       </c>
@@ -6103,10 +6103,10 @@
       <c r="I88" s="8"/>
     </row>
     <row r="89" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A89" s="25" t="s">
+      <c r="A89" s="35" t="s">
         <v>579</v>
       </c>
-      <c r="B89" s="25" t="s">
+      <c r="B89" s="35" t="s">
         <v>580</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -6130,8 +6130,8 @@
       <c r="I89" s="9"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26"/>
+      <c r="A90" s="36"/>
+      <c r="B90" s="36"/>
       <c r="C90" s="4" t="s">
         <v>564</v>
       </c>
@@ -6153,8 +6153,8 @@
       <c r="I90" s="9"/>
     </row>
     <row r="91" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
+      <c r="A91" s="36"/>
+      <c r="B91" s="36"/>
       <c r="C91" s="4" t="s">
         <v>582</v>
       </c>
@@ -6176,8 +6176,8 @@
       <c r="I91" s="9"/>
     </row>
     <row r="92" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
+      <c r="A92" s="36"/>
+      <c r="B92" s="36"/>
       <c r="C92" s="17" t="s">
         <v>571</v>
       </c>
@@ -6199,8 +6199,8 @@
       <c r="I92" s="9"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="27"/>
-      <c r="B93" s="27"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="37"/>
       <c r="C93" s="4" t="s">
         <v>569</v>
       </c>
@@ -6220,10 +6220,10 @@
       <c r="I93" s="9"/>
     </row>
     <row r="94" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A94" s="20" t="s">
+      <c r="A94" s="27" t="s">
         <v>574</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B94" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C94" s="5" t="s">
@@ -6249,8 +6249,8 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A95" s="20"/>
-      <c r="B95" s="20"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
       <c r="C95" s="5" t="s">
         <v>570</v>
       </c>
@@ -6272,8 +6272,8 @@
       <c r="I95" s="10"/>
     </row>
     <row r="96" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A96" s="20"/>
-      <c r="B96" s="20"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
       <c r="C96" s="5" t="s">
         <v>576</v>
       </c>
@@ -6295,8 +6295,8 @@
       <c r="I96" s="10"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="20"/>
-      <c r="B97" s="20"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
       <c r="C97" s="5" t="s">
         <v>577</v>
       </c>
@@ -6318,8 +6318,8 @@
       <c r="I97" s="10"/>
     </row>
     <row r="98" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A98" s="20"/>
-      <c r="B98" s="20"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
       <c r="C98" s="5" t="s">
         <v>578</v>
       </c>
@@ -6339,10 +6339,10 @@
       <c r="I98" s="10"/>
     </row>
     <row r="99" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A99" s="21" t="s">
+      <c r="A99" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="28" t="s">
         <v>359</v>
       </c>
       <c r="C99" s="6" t="s">
@@ -6366,8 +6366,8 @@
       <c r="I99" s="11"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="21"/>
-      <c r="B100" s="21"/>
+      <c r="A100" s="28"/>
+      <c r="B100" s="28"/>
       <c r="C100" s="6" t="s">
         <v>605</v>
       </c>
@@ -6387,8 +6387,8 @@
       <c r="I100" s="11"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="21"/>
-      <c r="B101" s="21"/>
+      <c r="A101" s="28"/>
+      <c r="B101" s="28"/>
       <c r="C101" s="6" t="s">
         <v>606</v>
       </c>
@@ -6408,8 +6408,8 @@
       <c r="I101" s="11"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="21"/>
-      <c r="B102" s="21"/>
+      <c r="A102" s="28"/>
+      <c r="B102" s="28"/>
       <c r="C102" s="6" t="s">
         <v>607</v>
       </c>
@@ -6429,8 +6429,8 @@
       <c r="I102" s="11"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="21"/>
-      <c r="B103" s="21"/>
+      <c r="A103" s="28"/>
+      <c r="B103" s="28"/>
       <c r="C103" s="6" t="s">
         <v>610</v>
       </c>
@@ -6450,10 +6450,10 @@
       <c r="I103" s="11"/>
     </row>
     <row r="104" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A104" s="28" t="s">
+      <c r="A104" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B104" s="28" t="s">
+      <c r="B104" s="22" t="s">
         <v>166</v>
       </c>
       <c r="C104" s="2" t="s">
@@ -6477,8 +6477,8 @@
       <c r="I104" s="7"/>
     </row>
     <row r="105" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A105" s="28"/>
-      <c r="B105" s="28"/>
+      <c r="A105" s="22"/>
+      <c r="B105" s="22"/>
       <c r="C105" s="2" t="s">
         <v>621</v>
       </c>
@@ -6500,8 +6500,8 @@
       <c r="I105" s="7"/>
     </row>
     <row r="106" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A106" s="28"/>
-      <c r="B106" s="28"/>
+      <c r="A106" s="22"/>
+      <c r="B106" s="22"/>
       <c r="C106" s="2" t="s">
         <v>627</v>
       </c>
@@ -6521,8 +6521,8 @@
       <c r="I106" s="7"/>
     </row>
     <row r="107" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="28"/>
-      <c r="B107" s="28"/>
+      <c r="A107" s="22"/>
+      <c r="B107" s="22"/>
       <c r="C107" s="2" t="s">
         <v>626</v>
       </c>
@@ -6544,8 +6544,8 @@
       <c r="I107" s="7"/>
     </row>
     <row r="108" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A108" s="28"/>
-      <c r="B108" s="28"/>
+      <c r="A108" s="22"/>
+      <c r="B108" s="22"/>
       <c r="C108" s="2" t="s">
         <v>46</v>
       </c>
@@ -6565,8 +6565,8 @@
       <c r="I108" s="7"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="28"/>
-      <c r="B109" s="28"/>
+      <c r="A109" s="22"/>
+      <c r="B109" s="22"/>
       <c r="C109" s="2" t="s">
         <v>619</v>
       </c>
@@ -6586,8 +6586,8 @@
       <c r="I109" s="7"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="28"/>
-      <c r="B110" s="28"/>
+      <c r="A110" s="22"/>
+      <c r="B110" s="22"/>
       <c r="C110" s="2" t="s">
         <v>620</v>
       </c>
@@ -6607,10 +6607,10 @@
       <c r="I110" s="7"/>
     </row>
     <row r="111" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A111" s="29" t="s">
+      <c r="A111" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B111" s="29" t="s">
+      <c r="B111" s="21" t="s">
         <v>167</v>
       </c>
       <c r="C111" s="3" t="s">
@@ -6634,8 +6634,8 @@
       <c r="I111" s="8"/>
     </row>
     <row r="112" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A112" s="29"/>
-      <c r="B112" s="29"/>
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
       <c r="C112" s="3" t="s">
         <v>632</v>
       </c>
@@ -6657,8 +6657,8 @@
       <c r="I112" s="8"/>
     </row>
     <row r="113" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A113" s="29"/>
-      <c r="B113" s="29"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="21"/>
       <c r="C113" s="3" t="s">
         <v>633</v>
       </c>
@@ -6678,8 +6678,8 @@
       <c r="I113" s="8"/>
     </row>
     <row r="114" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A114" s="29"/>
-      <c r="B114" s="29"/>
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
       <c r="C114" s="3" t="s">
         <v>634</v>
       </c>
@@ -6701,8 +6701,8 @@
       <c r="I114" s="8"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="29"/>
-      <c r="B115" s="29"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
       <c r="C115" s="3" t="s">
         <v>46</v>
       </c>
@@ -6722,8 +6722,8 @@
       <c r="I115" s="8"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="29"/>
-      <c r="B116" s="29"/>
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
       <c r="C116" s="3" t="s">
         <v>619</v>
       </c>
@@ -6743,8 +6743,8 @@
       <c r="I116" s="8"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="29"/>
-      <c r="B117" s="29"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="21"/>
       <c r="C117" s="3" t="s">
         <v>620</v>
       </c>
@@ -6764,10 +6764,10 @@
       <c r="I117" s="8"/>
     </row>
     <row r="118" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A118" s="30" t="s">
+      <c r="A118" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B118" s="30" t="s">
+      <c r="B118" s="26" t="s">
         <v>168</v>
       </c>
       <c r="C118" s="4" t="s">
@@ -6791,8 +6791,8 @@
       <c r="I118" s="9"/>
     </row>
     <row r="119" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A119" s="30"/>
-      <c r="B119" s="30"/>
+      <c r="A119" s="26"/>
+      <c r="B119" s="26"/>
       <c r="C119" s="4" t="s">
         <v>632</v>
       </c>
@@ -6814,8 +6814,8 @@
       <c r="I119" s="9"/>
     </row>
     <row r="120" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A120" s="30"/>
-      <c r="B120" s="30"/>
+      <c r="A120" s="26"/>
+      <c r="B120" s="26"/>
       <c r="C120" s="4" t="s">
         <v>633</v>
       </c>
@@ -6835,8 +6835,8 @@
       <c r="I120" s="9"/>
     </row>
     <row r="121" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A121" s="30"/>
-      <c r="B121" s="30"/>
+      <c r="A121" s="26"/>
+      <c r="B121" s="26"/>
       <c r="C121" s="4" t="s">
         <v>634</v>
       </c>
@@ -6858,8 +6858,8 @@
       <c r="I121" s="9"/>
     </row>
     <row r="122" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A122" s="30"/>
-      <c r="B122" s="30"/>
+      <c r="A122" s="26"/>
+      <c r="B122" s="26"/>
       <c r="C122" s="4" t="s">
         <v>46</v>
       </c>
@@ -6879,8 +6879,8 @@
       <c r="I122" s="9"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="30"/>
-      <c r="B123" s="30"/>
+      <c r="A123" s="26"/>
+      <c r="B123" s="26"/>
       <c r="C123" s="4" t="s">
         <v>619</v>
       </c>
@@ -6900,8 +6900,8 @@
       <c r="I123" s="9"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="30"/>
-      <c r="B124" s="30"/>
+      <c r="A124" s="26"/>
+      <c r="B124" s="26"/>
       <c r="C124" s="4" t="s">
         <v>620</v>
       </c>
@@ -6921,10 +6921,10 @@
       <c r="I124" s="9"/>
     </row>
     <row r="125" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A125" s="20" t="s">
+      <c r="A125" s="27" t="s">
         <v>667</v>
       </c>
-      <c r="B125" s="20" t="s">
+      <c r="B125" s="27" t="s">
         <v>668</v>
       </c>
       <c r="C125" s="5" t="s">
@@ -6948,8 +6948,8 @@
       <c r="I125" s="10"/>
     </row>
     <row r="126" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A126" s="20"/>
-      <c r="B126" s="20"/>
+      <c r="A126" s="27"/>
+      <c r="B126" s="27"/>
       <c r="C126" s="5" t="s">
         <v>250</v>
       </c>
@@ -6971,8 +6971,8 @@
       <c r="I126" s="10"/>
     </row>
     <row r="127" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A127" s="20"/>
-      <c r="B127" s="20"/>
+      <c r="A127" s="27"/>
+      <c r="B127" s="27"/>
       <c r="C127" s="5" t="s">
         <v>673</v>
       </c>
@@ -6994,8 +6994,8 @@
       <c r="I127" s="10"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="20"/>
-      <c r="B128" s="20"/>
+      <c r="A128" s="27"/>
+      <c r="B128" s="27"/>
       <c r="C128" s="5" t="s">
         <v>251</v>
       </c>
@@ -7015,10 +7015,10 @@
       <c r="I128" s="10"/>
     </row>
     <row r="129" spans="1:9" ht="165" x14ac:dyDescent="0.3">
-      <c r="A129" s="21" t="s">
+      <c r="A129" s="28" t="s">
         <v>661</v>
       </c>
-      <c r="B129" s="21" t="s">
+      <c r="B129" s="28" t="s">
         <v>44</v>
       </c>
       <c r="C129" s="6" t="s">
@@ -7042,8 +7042,8 @@
       <c r="I129" s="11"/>
     </row>
     <row r="130" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A130" s="21"/>
-      <c r="B130" s="21"/>
+      <c r="A130" s="28"/>
+      <c r="B130" s="28"/>
       <c r="C130" s="6" t="s">
         <v>684</v>
       </c>
@@ -7065,8 +7065,8 @@
       <c r="I130" s="11"/>
     </row>
     <row r="131" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A131" s="21"/>
-      <c r="B131" s="21"/>
+      <c r="A131" s="28"/>
+      <c r="B131" s="28"/>
       <c r="C131" s="6" t="s">
         <v>683</v>
       </c>
@@ -7088,8 +7088,8 @@
       <c r="I131" s="11"/>
     </row>
     <row r="132" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A132" s="21"/>
-      <c r="B132" s="21"/>
+      <c r="A132" s="28"/>
+      <c r="B132" s="28"/>
       <c r="C132" s="6" t="s">
         <v>253</v>
       </c>
@@ -7109,8 +7109,8 @@
       <c r="I132" s="11"/>
     </row>
     <row r="133" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A133" s="21"/>
-      <c r="B133" s="21"/>
+      <c r="A133" s="28"/>
+      <c r="B133" s="28"/>
       <c r="C133" s="6" t="s">
         <v>689</v>
       </c>
@@ -7130,8 +7130,8 @@
       <c r="I133" s="11"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" s="21"/>
-      <c r="B134" s="21"/>
+      <c r="A134" s="28"/>
+      <c r="B134" s="28"/>
       <c r="C134" s="6" t="s">
         <v>694</v>
       </c>
@@ -7151,10 +7151,10 @@
       <c r="I134" s="11"/>
     </row>
     <row r="135" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A135" s="28" t="s">
+      <c r="A135" s="22" t="s">
         <v>662</v>
       </c>
-      <c r="B135" s="28" t="s">
+      <c r="B135" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C135" s="2" t="s">
@@ -7178,8 +7178,8 @@
       <c r="I135" s="7"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A136" s="28"/>
-      <c r="B136" s="28"/>
+      <c r="A136" s="22"/>
+      <c r="B136" s="22"/>
       <c r="C136" s="2" t="s">
         <v>255</v>
       </c>
@@ -7199,8 +7199,8 @@
       <c r="I136" s="7"/>
     </row>
     <row r="137" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A137" s="28"/>
-      <c r="B137" s="28"/>
+      <c r="A137" s="22"/>
+      <c r="B137" s="22"/>
       <c r="C137" s="2" t="s">
         <v>702</v>
       </c>
@@ -7220,8 +7220,8 @@
       <c r="I137" s="7"/>
     </row>
     <row r="138" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A138" s="28"/>
-      <c r="B138" s="28"/>
+      <c r="A138" s="22"/>
+      <c r="B138" s="22"/>
       <c r="C138" s="2" t="s">
         <v>256</v>
       </c>
@@ -7241,10 +7241,10 @@
       <c r="I138" s="7"/>
     </row>
     <row r="139" spans="1:9" ht="198" x14ac:dyDescent="0.3">
-      <c r="A139" s="32" t="s">
+      <c r="A139" s="20" t="s">
         <v>663</v>
       </c>
-      <c r="B139" s="32" t="s">
+      <c r="B139" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C139" s="15" t="s">
@@ -7268,8 +7268,8 @@
       <c r="I139" s="16"/>
     </row>
     <row r="140" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A140" s="32"/>
-      <c r="B140" s="32"/>
+      <c r="A140" s="20"/>
+      <c r="B140" s="20"/>
       <c r="C140" s="15" t="s">
         <v>707</v>
       </c>
@@ -7291,8 +7291,8 @@
       <c r="I140" s="16"/>
     </row>
     <row r="141" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A141" s="32"/>
-      <c r="B141" s="32"/>
+      <c r="A141" s="20"/>
+      <c r="B141" s="20"/>
       <c r="C141" s="15" t="s">
         <v>665</v>
       </c>
@@ -7314,8 +7314,8 @@
       <c r="I141" s="16"/>
     </row>
     <row r="142" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A142" s="32"/>
-      <c r="B142" s="32"/>
+      <c r="A142" s="20"/>
+      <c r="B142" s="20"/>
       <c r="C142" s="15" t="s">
         <v>716</v>
       </c>
@@ -7337,8 +7337,8 @@
       <c r="I142" s="16"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A143" s="32"/>
-      <c r="B143" s="32"/>
+      <c r="A143" s="20"/>
+      <c r="B143" s="20"/>
       <c r="C143" s="15" t="s">
         <v>666</v>
       </c>
@@ -7358,10 +7358,10 @@
       <c r="I143" s="16"/>
     </row>
     <row r="144" spans="1:9" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A144" s="29" t="s">
+      <c r="A144" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B144" s="29" t="s">
+      <c r="B144" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C144" s="3" t="s">
@@ -7387,8 +7387,8 @@
       </c>
     </row>
     <row r="145" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A145" s="29"/>
-      <c r="B145" s="29"/>
+      <c r="A145" s="21"/>
+      <c r="B145" s="21"/>
       <c r="C145" s="3" t="s">
         <v>55</v>
       </c>
@@ -7410,8 +7410,8 @@
       <c r="I145" s="8"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A146" s="29"/>
-      <c r="B146" s="29"/>
+      <c r="A146" s="21"/>
+      <c r="B146" s="21"/>
       <c r="C146" s="3" t="s">
         <v>267</v>
       </c>
@@ -7431,8 +7431,8 @@
       <c r="I146" s="8"/>
     </row>
     <row r="147" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A147" s="29"/>
-      <c r="B147" s="29"/>
+      <c r="A147" s="21"/>
+      <c r="B147" s="21"/>
       <c r="C147" s="3" t="s">
         <v>373</v>
       </c>
@@ -7452,8 +7452,8 @@
       <c r="I147" s="8"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A148" s="29"/>
-      <c r="B148" s="29"/>
+      <c r="A148" s="21"/>
+      <c r="B148" s="21"/>
       <c r="C148" s="3" t="s">
         <v>56</v>
       </c>
@@ -7473,10 +7473,10 @@
       <c r="I148" s="8"/>
     </row>
     <row r="149" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A149" s="30" t="s">
+      <c r="A149" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="B149" s="30" t="s">
+      <c r="B149" s="26" t="s">
         <v>57</v>
       </c>
       <c r="C149" s="4" t="s">
@@ -7500,8 +7500,8 @@
       <c r="I149" s="9"/>
     </row>
     <row r="150" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A150" s="30"/>
-      <c r="B150" s="30"/>
+      <c r="A150" s="26"/>
+      <c r="B150" s="26"/>
       <c r="C150" s="4" t="s">
         <v>59</v>
       </c>
@@ -7523,8 +7523,8 @@
       <c r="I150" s="9"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A151" s="30"/>
-      <c r="B151" s="30"/>
+      <c r="A151" s="26"/>
+      <c r="B151" s="26"/>
       <c r="C151" s="4" t="s">
         <v>60</v>
       </c>
@@ -7544,8 +7544,8 @@
       <c r="I151" s="9"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A152" s="30"/>
-      <c r="B152" s="30"/>
+      <c r="A152" s="26"/>
+      <c r="B152" s="26"/>
       <c r="C152" s="4" t="s">
         <v>284</v>
       </c>
@@ -7565,8 +7565,8 @@
       <c r="I152" s="9"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A153" s="30"/>
-      <c r="B153" s="30"/>
+      <c r="A153" s="26"/>
+      <c r="B153" s="26"/>
       <c r="C153" s="4" t="s">
         <v>312</v>
       </c>
@@ -7747,10 +7747,10 @@
       <c r="I160" s="10"/>
     </row>
     <row r="161" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A161" s="21" t="s">
+      <c r="A161" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B161" s="21" t="s">
+      <c r="B161" s="28" t="s">
         <v>62</v>
       </c>
       <c r="C161" s="6" t="s">
@@ -7774,8 +7774,8 @@
       <c r="I161" s="11"/>
     </row>
     <row r="162" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A162" s="21"/>
-      <c r="B162" s="21"/>
+      <c r="A162" s="28"/>
+      <c r="B162" s="28"/>
       <c r="C162" s="6" t="s">
         <v>64</v>
       </c>
@@ -7797,8 +7797,8 @@
       <c r="I162" s="11"/>
     </row>
     <row r="163" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A163" s="21"/>
-      <c r="B163" s="21"/>
+      <c r="A163" s="28"/>
+      <c r="B163" s="28"/>
       <c r="C163" s="6" t="s">
         <v>300</v>
       </c>
@@ -7818,8 +7818,8 @@
       <c r="I163" s="11"/>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A164" s="21"/>
-      <c r="B164" s="21"/>
+      <c r="A164" s="28"/>
+      <c r="B164" s="28"/>
       <c r="C164" s="6" t="s">
         <v>65</v>
       </c>
@@ -7839,8 +7839,8 @@
       <c r="I164" s="11"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A165" s="21"/>
-      <c r="B165" s="21"/>
+      <c r="A165" s="28"/>
+      <c r="B165" s="28"/>
       <c r="C165" s="6" t="s">
         <v>294</v>
       </c>
@@ -7860,10 +7860,10 @@
       <c r="I165" s="11"/>
     </row>
     <row r="166" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A166" s="28" t="s">
+      <c r="A166" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B166" s="28" t="s">
+      <c r="B166" s="22" t="s">
         <v>67</v>
       </c>
       <c r="C166" s="2" t="s">
@@ -7887,8 +7887,8 @@
       <c r="I166" s="7"/>
     </row>
     <row r="167" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A167" s="28"/>
-      <c r="B167" s="28"/>
+      <c r="A167" s="22"/>
+      <c r="B167" s="22"/>
       <c r="C167" s="2" t="s">
         <v>69</v>
       </c>
@@ -7910,8 +7910,8 @@
       <c r="I167" s="7"/>
     </row>
     <row r="168" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A168" s="28"/>
-      <c r="B168" s="28"/>
+      <c r="A168" s="22"/>
+      <c r="B168" s="22"/>
       <c r="C168" s="2" t="s">
         <v>310</v>
       </c>
@@ -7931,8 +7931,8 @@
       <c r="I168" s="7"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A169" s="28"/>
-      <c r="B169" s="28"/>
+      <c r="A169" s="22"/>
+      <c r="B169" s="22"/>
       <c r="C169" s="2" t="s">
         <v>70</v>
       </c>
@@ -7952,8 +7952,8 @@
       <c r="I169" s="7"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A170" s="28"/>
-      <c r="B170" s="28"/>
+      <c r="A170" s="22"/>
+      <c r="B170" s="22"/>
       <c r="C170" s="2" t="s">
         <v>293</v>
       </c>
@@ -7973,10 +7973,10 @@
       <c r="I170" s="7"/>
     </row>
     <row r="171" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A171" s="29" t="s">
+      <c r="A171" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="B171" s="29" t="s">
+      <c r="B171" s="21" t="s">
         <v>283</v>
       </c>
       <c r="C171" s="3" t="s">
@@ -8000,8 +8000,8 @@
       <c r="I171" s="8"/>
     </row>
     <row r="172" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A172" s="29"/>
-      <c r="B172" s="29"/>
+      <c r="A172" s="21"/>
+      <c r="B172" s="21"/>
       <c r="C172" s="3" t="s">
         <v>72</v>
       </c>
@@ -8023,8 +8023,8 @@
       <c r="I172" s="8"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A173" s="29"/>
-      <c r="B173" s="29"/>
+      <c r="A173" s="21"/>
+      <c r="B173" s="21"/>
       <c r="C173" s="3" t="s">
         <v>348</v>
       </c>
@@ -8044,8 +8044,8 @@
       <c r="I173" s="8"/>
     </row>
     <row r="174" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A174" s="29"/>
-      <c r="B174" s="29"/>
+      <c r="A174" s="21"/>
+      <c r="B174" s="21"/>
       <c r="C174" s="3" t="s">
         <v>73</v>
       </c>
@@ -8065,8 +8065,8 @@
       <c r="I174" s="8"/>
     </row>
     <row r="175" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A175" s="29"/>
-      <c r="B175" s="29"/>
+      <c r="A175" s="21"/>
+      <c r="B175" s="21"/>
       <c r="C175" s="3" t="s">
         <v>347</v>
       </c>
@@ -8086,10 +8086,10 @@
       <c r="I175" s="8"/>
     </row>
     <row r="176" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A176" s="22" t="s">
+      <c r="A176" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B176" s="22" t="s">
+      <c r="B176" s="29" t="s">
         <v>356</v>
       </c>
       <c r="C176" s="15" t="s">
@@ -8113,8 +8113,8 @@
       <c r="I176" s="14"/>
     </row>
     <row r="177" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A177" s="23"/>
-      <c r="B177" s="23"/>
+      <c r="A177" s="30"/>
+      <c r="B177" s="30"/>
       <c r="C177" s="15" t="s">
         <v>76</v>
       </c>
@@ -8134,8 +8134,8 @@
       <c r="I177" s="14"/>
     </row>
     <row r="178" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A178" s="23"/>
-      <c r="B178" s="23"/>
+      <c r="A178" s="30"/>
+      <c r="B178" s="30"/>
       <c r="C178" s="15" t="s">
         <v>77</v>
       </c>
@@ -8155,8 +8155,8 @@
       <c r="I178" s="14"/>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A179" s="24"/>
-      <c r="B179" s="24"/>
+      <c r="A179" s="31"/>
+      <c r="B179" s="31"/>
       <c r="C179" s="15" t="s">
         <v>726</v>
       </c>
@@ -8176,10 +8176,10 @@
       <c r="I179" s="16"/>
     </row>
     <row r="180" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A180" s="30" t="s">
+      <c r="A180" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B180" s="30" t="s">
+      <c r="B180" s="26" t="s">
         <v>79</v>
       </c>
       <c r="C180" s="4" t="s">
@@ -8203,8 +8203,8 @@
       <c r="I180" s="9"/>
     </row>
     <row r="181" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A181" s="30"/>
-      <c r="B181" s="30"/>
+      <c r="A181" s="26"/>
+      <c r="B181" s="26"/>
       <c r="C181" s="4" t="s">
         <v>81</v>
       </c>
@@ -8226,8 +8226,8 @@
       <c r="I181" s="9"/>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A182" s="30"/>
-      <c r="B182" s="30"/>
+      <c r="A182" s="26"/>
+      <c r="B182" s="26"/>
       <c r="C182" s="4" t="s">
         <v>364</v>
       </c>
@@ -8247,8 +8247,8 @@
       <c r="I182" s="9"/>
     </row>
     <row r="183" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A183" s="30"/>
-      <c r="B183" s="30"/>
+      <c r="A183" s="26"/>
+      <c r="B183" s="26"/>
       <c r="C183" s="4" t="s">
         <v>374</v>
       </c>
@@ -8268,8 +8268,8 @@
       <c r="I183" s="9"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A184" s="30"/>
-      <c r="B184" s="30"/>
+      <c r="A184" s="26"/>
+      <c r="B184" s="26"/>
       <c r="C184" s="4" t="s">
         <v>82</v>
       </c>
@@ -8289,10 +8289,10 @@
       <c r="I184" s="9"/>
     </row>
     <row r="185" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A185" s="20" t="s">
+      <c r="A185" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B185" s="20" t="s">
+      <c r="B185" s="27" t="s">
         <v>105</v>
       </c>
       <c r="C185" s="5" t="s">
@@ -8316,8 +8316,8 @@
       <c r="I185" s="10"/>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A186" s="20"/>
-      <c r="B186" s="20"/>
+      <c r="A186" s="27"/>
+      <c r="B186" s="27"/>
       <c r="C186" s="5" t="s">
         <v>85</v>
       </c>
@@ -8337,10 +8337,10 @@
       <c r="I186" s="10"/>
     </row>
     <row r="187" spans="1:9" ht="231" x14ac:dyDescent="0.3">
-      <c r="A187" s="22" t="s">
+      <c r="A187" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B187" s="22" t="s">
+      <c r="B187" s="29" t="s">
         <v>405</v>
       </c>
       <c r="C187" s="15" t="s">
@@ -8364,8 +8364,8 @@
       <c r="I187" s="14"/>
     </row>
     <row r="188" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A188" s="23"/>
-      <c r="B188" s="23"/>
+      <c r="A188" s="30"/>
+      <c r="B188" s="30"/>
       <c r="C188" s="15" t="s">
         <v>89</v>
       </c>
@@ -8387,8 +8387,8 @@
       <c r="I188" s="14"/>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A189" s="23"/>
-      <c r="B189" s="23"/>
+      <c r="A189" s="30"/>
+      <c r="B189" s="30"/>
       <c r="C189" s="15" t="s">
         <v>383</v>
       </c>
@@ -8408,8 +8408,8 @@
       <c r="I189" s="14"/>
     </row>
     <row r="190" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A190" s="23"/>
-      <c r="B190" s="23"/>
+      <c r="A190" s="30"/>
+      <c r="B190" s="30"/>
       <c r="C190" s="15" t="s">
         <v>406</v>
       </c>
@@ -8429,8 +8429,8 @@
       <c r="I190" s="14"/>
     </row>
     <row r="191" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A191" s="23"/>
-      <c r="B191" s="23"/>
+      <c r="A191" s="30"/>
+      <c r="B191" s="30"/>
       <c r="C191" s="15" t="s">
         <v>411</v>
       </c>
@@ -8452,8 +8452,8 @@
       <c r="I191" s="14"/>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A192" s="23"/>
-      <c r="B192" s="23"/>
+      <c r="A192" s="30"/>
+      <c r="B192" s="30"/>
       <c r="C192" s="15" t="s">
         <v>90</v>
       </c>
@@ -8473,8 +8473,8 @@
       <c r="I192" s="14"/>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A193" s="24"/>
-      <c r="B193" s="24"/>
+      <c r="A193" s="31"/>
+      <c r="B193" s="31"/>
       <c r="C193" s="15" t="s">
         <v>732</v>
       </c>
@@ -8494,10 +8494,10 @@
       <c r="I193" s="16"/>
     </row>
     <row r="194" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A194" s="31" t="s">
+      <c r="A194" s="34" t="s">
         <v>390</v>
       </c>
-      <c r="B194" s="31" t="s">
+      <c r="B194" s="34" t="s">
         <v>83</v>
       </c>
       <c r="C194" s="13" t="s">
@@ -8521,8 +8521,8 @@
       <c r="I194" s="12"/>
     </row>
     <row r="195" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A195" s="31"/>
-      <c r="B195" s="31"/>
+      <c r="A195" s="34"/>
+      <c r="B195" s="34"/>
       <c r="C195" s="13" t="s">
         <v>92</v>
       </c>
@@ -8544,8 +8544,8 @@
       <c r="I195" s="12"/>
     </row>
     <row r="196" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A196" s="31"/>
-      <c r="B196" s="31"/>
+      <c r="A196" s="34"/>
+      <c r="B196" s="34"/>
       <c r="C196" s="13" t="s">
         <v>391</v>
       </c>
@@ -8565,8 +8565,8 @@
       <c r="I196" s="12"/>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A197" s="31"/>
-      <c r="B197" s="31"/>
+      <c r="A197" s="34"/>
+      <c r="B197" s="34"/>
       <c r="C197" s="13" t="s">
         <v>93</v>
       </c>
@@ -8586,8 +8586,8 @@
       <c r="I197" s="12"/>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A198" s="31"/>
-      <c r="B198" s="31"/>
+      <c r="A198" s="34"/>
+      <c r="B198" s="34"/>
       <c r="C198" s="13" t="s">
         <v>392</v>
       </c>
@@ -8607,10 +8607,10 @@
       <c r="I198" s="12"/>
     </row>
     <row r="199" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A199" s="32" t="s">
+      <c r="A199" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="B199" s="32" t="s">
+      <c r="B199" s="20" t="s">
         <v>87</v>
       </c>
       <c r="C199" s="15" t="s">
@@ -8634,8 +8634,8 @@
       <c r="I199" s="14"/>
     </row>
     <row r="200" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A200" s="32"/>
-      <c r="B200" s="32"/>
+      <c r="A200" s="20"/>
+      <c r="B200" s="20"/>
       <c r="C200" s="15" t="s">
         <v>107</v>
       </c>
@@ -8657,8 +8657,8 @@
       <c r="I200" s="14"/>
     </row>
     <row r="201" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A201" s="32"/>
-      <c r="B201" s="32"/>
+      <c r="A201" s="20"/>
+      <c r="B201" s="20"/>
       <c r="C201" s="15" t="s">
         <v>403</v>
       </c>
@@ -8678,8 +8678,8 @@
       <c r="I201" s="14"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" s="32"/>
-      <c r="B202" s="32"/>
+      <c r="A202" s="20"/>
+      <c r="B202" s="20"/>
       <c r="C202" s="15" t="s">
         <v>108</v>
       </c>
@@ -8699,8 +8699,8 @@
       <c r="I202" s="14"/>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A203" s="32"/>
-      <c r="B203" s="32"/>
+      <c r="A203" s="20"/>
+      <c r="B203" s="20"/>
       <c r="C203" s="15" t="s">
         <v>404</v>
       </c>
@@ -8720,10 +8720,10 @@
       <c r="I203" s="14"/>
     </row>
     <row r="204" spans="1:9" ht="165" x14ac:dyDescent="0.3">
-      <c r="A204" s="21" t="s">
+      <c r="A204" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B204" s="21" t="s">
+      <c r="B204" s="28" t="s">
         <v>95</v>
       </c>
       <c r="C204" s="6" t="s">
@@ -8749,8 +8749,8 @@
       </c>
     </row>
     <row r="205" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A205" s="21"/>
-      <c r="B205" s="21"/>
+      <c r="A205" s="28"/>
+      <c r="B205" s="28"/>
       <c r="C205" s="6" t="s">
         <v>97</v>
       </c>
@@ -8772,8 +8772,8 @@
       <c r="I205" s="11"/>
     </row>
     <row r="206" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A206" s="21"/>
-      <c r="B206" s="21"/>
+      <c r="A206" s="28"/>
+      <c r="B206" s="28"/>
       <c r="C206" s="6" t="s">
         <v>98</v>
       </c>
@@ -8793,8 +8793,8 @@
       <c r="I206" s="11"/>
     </row>
     <row r="207" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A207" s="21"/>
-      <c r="B207" s="21"/>
+      <c r="A207" s="28"/>
+      <c r="B207" s="28"/>
       <c r="C207" s="6" t="s">
         <v>427</v>
       </c>
@@ -8814,10 +8814,10 @@
       <c r="I207" s="11"/>
     </row>
     <row r="208" spans="1:9" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A208" s="22" t="s">
+      <c r="A208" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B208" s="22" t="s">
+      <c r="B208" s="29" t="s">
         <v>100</v>
       </c>
       <c r="C208" s="15" t="s">
@@ -8841,8 +8841,8 @@
       <c r="I208" s="14"/>
     </row>
     <row r="209" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A209" s="23"/>
-      <c r="B209" s="23"/>
+      <c r="A209" s="30"/>
+      <c r="B209" s="30"/>
       <c r="C209" s="15" t="s">
         <v>102</v>
       </c>
@@ -8862,8 +8862,8 @@
       <c r="I209" s="14"/>
     </row>
     <row r="210" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A210" s="23"/>
-      <c r="B210" s="23"/>
+      <c r="A210" s="30"/>
+      <c r="B210" s="30"/>
       <c r="C210" s="15" t="s">
         <v>432</v>
       </c>
@@ -8883,8 +8883,8 @@
       <c r="I210" s="14"/>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A211" s="23"/>
-      <c r="B211" s="23"/>
+      <c r="A211" s="30"/>
+      <c r="B211" s="30"/>
       <c r="C211" s="15" t="s">
         <v>103</v>
       </c>
@@ -8904,8 +8904,8 @@
       <c r="I211" s="14"/>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A212" s="24"/>
-      <c r="B212" s="24"/>
+      <c r="A212" s="31"/>
+      <c r="B212" s="31"/>
       <c r="C212" s="15" t="s">
         <v>727</v>
       </c>
@@ -8925,10 +8925,10 @@
       <c r="I212" s="16"/>
     </row>
     <row r="213" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A213" s="28" t="s">
+      <c r="A213" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B213" s="28" t="s">
+      <c r="B213" s="22" t="s">
         <v>110</v>
       </c>
       <c r="C213" s="2" t="s">
@@ -8954,8 +8954,8 @@
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A214" s="28"/>
-      <c r="B214" s="28"/>
+      <c r="A214" s="22"/>
+      <c r="B214" s="22"/>
       <c r="C214" s="2" t="s">
         <v>112</v>
       </c>
@@ -8975,10 +8975,10 @@
       <c r="I214" s="7"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A215" s="29" t="s">
+      <c r="A215" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B215" s="29" t="s">
+      <c r="B215" s="21" t="s">
         <v>117</v>
       </c>
       <c r="C215" s="3" t="s">
@@ -9002,8 +9002,8 @@
       <c r="I215" s="8"/>
     </row>
     <row r="216" spans="1:9" ht="99" x14ac:dyDescent="0.3">
-      <c r="A216" s="29"/>
-      <c r="B216" s="29"/>
+      <c r="A216" s="21"/>
+      <c r="B216" s="21"/>
       <c r="C216" s="3" t="s">
         <v>468</v>
       </c>
@@ -9027,8 +9027,8 @@
       </c>
     </row>
     <row r="217" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A217" s="29"/>
-      <c r="B217" s="29"/>
+      <c r="A217" s="21"/>
+      <c r="B217" s="21"/>
       <c r="C217" s="3" t="s">
         <v>115</v>
       </c>
@@ -9048,8 +9048,8 @@
       <c r="I217" s="8"/>
     </row>
     <row r="218" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A218" s="29"/>
-      <c r="B218" s="29"/>
+      <c r="A218" s="21"/>
+      <c r="B218" s="21"/>
       <c r="C218" s="3" t="s">
         <v>476</v>
       </c>
@@ -9069,8 +9069,8 @@
       <c r="I218" s="8"/>
     </row>
     <row r="219" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A219" s="29"/>
-      <c r="B219" s="29"/>
+      <c r="A219" s="21"/>
+      <c r="B219" s="21"/>
       <c r="C219" s="3" t="s">
         <v>116</v>
       </c>
@@ -9090,8 +9090,8 @@
       <c r="I219" s="8"/>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A220" s="29"/>
-      <c r="B220" s="29"/>
+      <c r="A220" s="21"/>
+      <c r="B220" s="21"/>
       <c r="C220" s="3" t="s">
         <v>475</v>
       </c>
@@ -9112,31 +9112,36 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B139:B143"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="B111:B117"/>
-    <mergeCell ref="B118:B124"/>
-    <mergeCell ref="A72:A76"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A59:A65"/>
-    <mergeCell ref="B59:B65"/>
-    <mergeCell ref="A66:A71"/>
-    <mergeCell ref="B66:B71"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="B2:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B37:B44"/>
+    <mergeCell ref="A176:A179"/>
+    <mergeCell ref="B176:B179"/>
+    <mergeCell ref="B149:B153"/>
+    <mergeCell ref="B161:B165"/>
+    <mergeCell ref="B166:B170"/>
+    <mergeCell ref="A161:A165"/>
+    <mergeCell ref="A149:A153"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="A125:A128"/>
+    <mergeCell ref="B125:B128"/>
+    <mergeCell ref="A215:A220"/>
+    <mergeCell ref="B215:B220"/>
+    <mergeCell ref="A180:A184"/>
+    <mergeCell ref="B180:B184"/>
+    <mergeCell ref="A194:A198"/>
+    <mergeCell ref="B194:B198"/>
+    <mergeCell ref="A199:A203"/>
+    <mergeCell ref="B199:B203"/>
+    <mergeCell ref="A185:A186"/>
+    <mergeCell ref="B185:B186"/>
+    <mergeCell ref="A187:A193"/>
+    <mergeCell ref="B187:B193"/>
+    <mergeCell ref="A208:A212"/>
+    <mergeCell ref="B208:B212"/>
+    <mergeCell ref="A204:A207"/>
+    <mergeCell ref="B204:B207"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="A21:A28"/>
     <mergeCell ref="B21:B28"/>
@@ -9153,42 +9158,37 @@
     <mergeCell ref="A29:A36"/>
     <mergeCell ref="B29:B36"/>
     <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A215:A220"/>
-    <mergeCell ref="B215:B220"/>
-    <mergeCell ref="A180:A184"/>
-    <mergeCell ref="B180:B184"/>
-    <mergeCell ref="A194:A198"/>
-    <mergeCell ref="B194:B198"/>
-    <mergeCell ref="A199:A203"/>
-    <mergeCell ref="B199:B203"/>
-    <mergeCell ref="A185:A186"/>
-    <mergeCell ref="B185:B186"/>
-    <mergeCell ref="A187:A193"/>
-    <mergeCell ref="B187:B193"/>
-    <mergeCell ref="A208:A212"/>
-    <mergeCell ref="B208:B212"/>
-    <mergeCell ref="A204:A207"/>
-    <mergeCell ref="B204:B207"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="B2:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B37:B44"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="B111:B117"/>
+    <mergeCell ref="B118:B124"/>
+    <mergeCell ref="A72:A76"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A59:A65"/>
+    <mergeCell ref="B59:B65"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="B66:B71"/>
     <mergeCell ref="A89:A93"/>
     <mergeCell ref="B89:B93"/>
     <mergeCell ref="A104:A110"/>
     <mergeCell ref="B104:B110"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="A125:A128"/>
-    <mergeCell ref="B125:B128"/>
+    <mergeCell ref="B139:B143"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="B80:B84"/>
     <mergeCell ref="A129:A134"/>
     <mergeCell ref="B129:B134"/>
-    <mergeCell ref="A176:A179"/>
-    <mergeCell ref="B176:B179"/>
-    <mergeCell ref="B149:B153"/>
-    <mergeCell ref="B161:B165"/>
-    <mergeCell ref="B166:B170"/>
-    <mergeCell ref="A161:A165"/>
-    <mergeCell ref="A149:A153"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B154:B160"/>
     <mergeCell ref="A135:A138"/>
     <mergeCell ref="A139:A143"/>
     <mergeCell ref="B135:B138"/>

</xml_diff>

<commit_message>
0616 (요구정의서, user, login, signup, errormsg) 이가원
</commit_message>
<xml_diff>
--- a/docs/요구사항정의서.xlsx
+++ b/docs/요구사항정의서.xlsx
@@ -3844,7 +3844,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3917,6 +3917,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3984,7 +3990,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4042,7 +4048,118 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4057,119 +4174,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4454,8 +4466,8 @@
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J220"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F181" sqref="F181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4505,13 +4517,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="54" t="s">
         <v>765</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4537,9 +4549,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
@@ -4559,9 +4571,9 @@
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>133</v>
       </c>
@@ -4581,9 +4593,9 @@
       <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>136</v>
       </c>
@@ -4603,9 +4615,9 @@
       <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="2" t="s">
         <v>140</v>
       </c>
@@ -4625,125 +4637,125 @@
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="59" t="s">
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="56" t="s">
         <v>768</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="20">
         <v>1</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J7" s="43"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="42" t="s">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="19" t="s">
         <v>756</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="20">
         <v>1</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J8" s="43"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="42" t="s">
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43">
+      <c r="G9" s="19"/>
+      <c r="H9" s="20">
         <v>1</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J9" s="43"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="42" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="43">
+      <c r="G10" s="19"/>
+      <c r="H10" s="20">
         <v>1</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J10" s="43"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="42" t="s">
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43">
+      <c r="G11" s="19"/>
+      <c r="H11" s="20">
         <v>3</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J11" s="43"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54" t="s">
         <v>783</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -4767,9 +4779,9 @@
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="2" t="s">
         <v>126</v>
       </c>
@@ -4791,9 +4803,9 @@
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="2" t="s">
         <v>156</v>
       </c>
@@ -4813,59 +4825,59 @@
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="59" t="s">
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="56" t="s">
         <v>764</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H15" s="20">
         <v>3</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J15" s="43"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="42" t="s">
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="19" t="s">
         <v>758</v>
       </c>
-      <c r="H16" s="43">
+      <c r="H16" s="20">
         <v>3</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="J16" s="43"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25" t="s">
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54" t="s">
         <v>767</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -4889,9 +4901,9 @@
       <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="2" t="s">
         <v>291</v>
       </c>
@@ -4913,13 +4925,13 @@
       <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="55" t="s">
         <v>769</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -4943,9 +4955,9 @@
       <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="3" t="s">
         <v>14</v>
       </c>
@@ -4965,13 +4977,13 @@
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="46" t="s">
         <v>771</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -4997,9 +5009,9 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="4" t="s">
         <v>16</v>
       </c>
@@ -5019,9 +5031,9 @@
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
@@ -5041,9 +5053,9 @@
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="4" t="s">
         <v>177</v>
       </c>
@@ -5063,59 +5075,59 @@
       <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="53" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="51" t="s">
         <v>772</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="24" t="s">
         <v>823</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="F25" s="55" t="s">
+      <c r="F25" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="G25" s="55" t="s">
+      <c r="G25" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="H25" s="54">
+      <c r="H25" s="23">
         <v>2</v>
       </c>
-      <c r="I25" s="54" t="s">
+      <c r="I25" s="23" t="s">
         <v>470</v>
       </c>
-      <c r="J25" s="53" t="s">
+      <c r="J25" s="51" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="55" t="s">
+      <c r="A26" s="46"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="F26" s="55" t="s">
+      <c r="F26" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="G26" s="55"/>
-      <c r="H26" s="54">
+      <c r="G26" s="24"/>
+      <c r="H26" s="23">
         <v>2</v>
       </c>
-      <c r="I26" s="54" t="s">
+      <c r="I26" s="23" t="s">
         <v>470</v>
       </c>
-      <c r="J26" s="53"/>
+      <c r="J26" s="51"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30" t="s">
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46" t="s">
         <v>773</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -5136,14 +5148,14 @@
       <c r="I27" s="14" t="s">
         <v>470</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="46" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="4" t="s">
         <v>187</v>
       </c>
@@ -5160,16 +5172,16 @@
       <c r="I28" s="14" t="s">
         <v>470</v>
       </c>
-      <c r="J28" s="30"/>
+      <c r="J28" s="46"/>
     </row>
     <row r="29" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="52" t="s">
         <v>775</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -5193,9 +5205,9 @@
       <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
       <c r="D30" s="5" t="s">
         <v>148</v>
       </c>
@@ -5215,9 +5227,9 @@
       <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
       <c r="D31" s="5" t="s">
         <v>149</v>
       </c>
@@ -5237,9 +5249,9 @@
       <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="5" t="s">
         <v>199</v>
       </c>
@@ -5259,105 +5271,105 @@
       <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="52" t="s">
+      <c r="A33" s="52"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53" t="s">
         <v>776</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="21" t="s">
         <v>774</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="H33" s="47">
+      <c r="H33" s="22">
         <v>4</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="I33" s="22" t="s">
         <v>470</v>
       </c>
-      <c r="J33" s="47"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="46" t="s">
+      <c r="A34" s="52"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E34" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="G34" s="46"/>
-      <c r="H34" s="47">
+      <c r="G34" s="21"/>
+      <c r="H34" s="22">
         <v>4</v>
       </c>
-      <c r="I34" s="47" t="s">
+      <c r="I34" s="22" t="s">
         <v>470</v>
       </c>
-      <c r="J34" s="47"/>
+      <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="46" t="s">
+      <c r="A35" s="52"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="F35" s="46" t="s">
+      <c r="F35" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="G35" s="46"/>
-      <c r="H35" s="47">
+      <c r="G35" s="21"/>
+      <c r="H35" s="22">
         <v>4</v>
       </c>
-      <c r="I35" s="47" t="s">
+      <c r="I35" s="22" t="s">
         <v>470</v>
       </c>
-      <c r="J35" s="47"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="46" t="s">
+      <c r="A36" s="52"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="F36" s="46" t="s">
+      <c r="F36" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="G36" s="46"/>
-      <c r="H36" s="47">
+      <c r="G36" s="21"/>
+      <c r="H36" s="22">
         <v>4</v>
       </c>
-      <c r="I36" s="47" t="s">
+      <c r="I36" s="22" t="s">
         <v>470</v>
       </c>
-      <c r="J36" s="47"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="50" t="s">
         <v>777</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -5383,9 +5395,9 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="6" t="s">
         <v>20</v>
       </c>
@@ -5405,9 +5417,9 @@
       <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="6" t="s">
         <v>21</v>
       </c>
@@ -5427,9 +5439,9 @@
       <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="6" t="s">
         <v>212</v>
       </c>
@@ -5449,9 +5461,9 @@
       <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="6" t="s">
         <v>215</v>
       </c>
@@ -5471,9 +5483,9 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="6" t="s">
         <v>219</v>
       </c>
@@ -5495,9 +5507,9 @@
       <c r="J42" s="15"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="6" t="s">
         <v>222</v>
       </c>
@@ -5519,9 +5531,9 @@
       <c r="J43" s="15"/>
     </row>
     <row r="44" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="50"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="6" t="s">
         <v>218</v>
       </c>
@@ -5541,13 +5553,13 @@
       <c r="J44" s="15"/>
     </row>
     <row r="45" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C45" s="30" t="s">
         <v>778</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -5571,9 +5583,9 @@
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="39"/>
+      <c r="A46" s="54"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="2" t="s">
         <v>29</v>
       </c>
@@ -5593,57 +5605,57 @@
       <c r="J46" s="16"/>
     </row>
     <row r="47" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="41" t="s">
+      <c r="A47" s="54"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="36" t="s">
         <v>818</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D47" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="E47" s="42" t="s">
+      <c r="E47" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="F47" s="42" t="s">
+      <c r="F47" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="G47" s="42" t="s">
+      <c r="G47" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="H47" s="43">
+      <c r="H47" s="20">
         <v>2</v>
       </c>
-      <c r="I47" s="43" t="s">
+      <c r="I47" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="J47" s="43"/>
+      <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="42" t="s">
+      <c r="A48" s="54"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="19" t="s">
         <v>743</v>
       </c>
-      <c r="E48" s="42" t="s">
+      <c r="E48" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="F48" s="42" t="s">
+      <c r="F48" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="43">
+      <c r="G48" s="19"/>
+      <c r="H48" s="20">
         <v>2</v>
       </c>
-      <c r="I48" s="43" t="s">
+      <c r="I48" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="J48" s="43"/>
+      <c r="J48" s="20"/>
     </row>
     <row r="49" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="38" t="s">
+      <c r="A49" s="54"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="30" t="s">
         <v>802</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -5667,9 +5679,9 @@
       <c r="J49" s="16"/>
     </row>
     <row r="50" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="39"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="2" t="s">
         <v>742</v>
       </c>
@@ -5689,39 +5701,39 @@
       <c r="J50" s="16"/>
     </row>
     <row r="51" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="43" t="s">
+      <c r="A51" s="54"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="20" t="s">
         <v>819</v>
       </c>
-      <c r="D51" s="42" t="s">
+      <c r="D51" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="E51" s="42" t="s">
+      <c r="E51" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="F51" s="42" t="s">
+      <c r="F51" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="G51" s="42" t="s">
+      <c r="G51" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="H51" s="43">
+      <c r="H51" s="20">
         <v>4</v>
       </c>
-      <c r="I51" s="43" t="s">
+      <c r="I51" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="J51" s="43"/>
+      <c r="J51" s="20"/>
     </row>
     <row r="52" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="55" t="s">
         <v>314</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="55" t="s">
         <v>317</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="C52" s="33" t="s">
         <v>779</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -5745,9 +5757,9 @@
       <c r="J52" s="18"/>
     </row>
     <row r="53" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="55"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="34"/>
       <c r="D53" s="3" t="s">
         <v>755</v>
       </c>
@@ -5769,9 +5781,9 @@
       <c r="J53" s="18"/>
     </row>
     <row r="54" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="55"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="34"/>
       <c r="D54" s="3" t="s">
         <v>319</v>
       </c>
@@ -5793,9 +5805,9 @@
       <c r="J54" s="18"/>
     </row>
     <row r="55" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="28"/>
+      <c r="A55" s="55"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="34"/>
       <c r="D55" s="3" t="s">
         <v>320</v>
       </c>
@@ -5817,9 +5829,9 @@
       <c r="J55" s="18"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="28"/>
+      <c r="A56" s="55"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="34"/>
       <c r="D56" s="3" t="s">
         <v>321</v>
       </c>
@@ -5839,9 +5851,9 @@
       <c r="J56" s="18"/>
     </row>
     <row r="57" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="28"/>
+      <c r="A57" s="55"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="34"/>
       <c r="D57" s="3" t="s">
         <v>322</v>
       </c>
@@ -5863,9 +5875,9 @@
       <c r="J57" s="18"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="29"/>
+      <c r="A58" s="55"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="3" t="s">
         <v>323</v>
       </c>
@@ -5885,13 +5897,13 @@
       <c r="J58" s="18"/>
     </row>
     <row r="59" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="38" t="s">
         <v>781</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5917,9 +5929,9 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="33"/>
+      <c r="A60" s="46"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="39"/>
       <c r="D60" s="4" t="s">
         <v>50</v>
       </c>
@@ -5939,9 +5951,9 @@
       <c r="J60" s="14"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="34"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="40"/>
       <c r="D61" s="4" t="s">
         <v>51</v>
       </c>
@@ -5961,61 +5973,61 @@
       <c r="J61" s="14"/>
     </row>
     <row r="62" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="56" t="s">
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="47" t="s">
         <v>782</v>
       </c>
-      <c r="D62" s="55" t="s">
+      <c r="D62" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="F62" s="55" t="s">
+      <c r="F62" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="G62" s="55" t="s">
+      <c r="G62" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="H62" s="54">
+      <c r="H62" s="23">
         <v>3</v>
       </c>
-      <c r="I62" s="54" t="s">
+      <c r="I62" s="23" t="s">
         <v>472</v>
       </c>
-      <c r="J62" s="54"/>
+      <c r="J62" s="23"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="30"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="55" t="s">
+      <c r="A63" s="46"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="E63" s="55" t="s">
+      <c r="E63" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="F63" s="55" t="s">
+      <c r="F63" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="G63" s="55"/>
-      <c r="H63" s="54">
+      <c r="G63" s="24"/>
+      <c r="H63" s="23">
         <v>3</v>
       </c>
-      <c r="I63" s="54" t="s">
+      <c r="I63" s="23" t="s">
         <v>472</v>
       </c>
-      <c r="J63" s="54"/>
+      <c r="J63" s="23"/>
     </row>
     <row r="64" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="52" t="s">
         <v>301</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="43" t="s">
         <v>780</v>
       </c>
       <c r="D64" s="5" t="s">
@@ -6039,9 +6051,9 @@
       <c r="J64" s="17"/>
     </row>
     <row r="65" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="31"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="36"/>
+      <c r="A65" s="52"/>
+      <c r="B65" s="52"/>
+      <c r="C65" s="44"/>
       <c r="D65" s="5" t="s">
         <v>54</v>
       </c>
@@ -6063,9 +6075,9 @@
       <c r="J65" s="17"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="31"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="36"/>
+      <c r="A66" s="52"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="44"/>
       <c r="D66" s="5" t="s">
         <v>55</v>
       </c>
@@ -6085,9 +6097,9 @@
       <c r="J66" s="17"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="31"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="36"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="52"/>
+      <c r="C67" s="44"/>
       <c r="D67" s="5" t="s">
         <v>275</v>
       </c>
@@ -6107,9 +6119,9 @@
       <c r="J67" s="17"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="31"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="37"/>
+      <c r="A68" s="52"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="45"/>
       <c r="D68" s="5" t="s">
         <v>302</v>
       </c>
@@ -6129,13 +6141,13 @@
       <c r="J68" s="17"/>
     </row>
     <row r="69" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="50" t="s">
         <v>316</v>
       </c>
-      <c r="B69" s="26" t="s">
+      <c r="B69" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="C69" s="49" t="s">
+      <c r="C69" s="27" t="s">
         <v>784</v>
       </c>
       <c r="D69" s="6" t="s">
@@ -6159,9 +6171,9 @@
       <c r="J69" s="15"/>
     </row>
     <row r="70" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="50"/>
+      <c r="A70" s="50"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="28"/>
       <c r="D70" s="6" t="s">
         <v>747</v>
       </c>
@@ -6183,9 +6195,9 @@
       <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="50"/>
+      <c r="A71" s="50"/>
+      <c r="B71" s="50"/>
+      <c r="C71" s="28"/>
       <c r="D71" s="6" t="s">
         <v>325</v>
       </c>
@@ -6207,9 +6219,9 @@
       <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="50"/>
+      <c r="A72" s="50"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="28"/>
       <c r="D72" s="6" t="s">
         <v>326</v>
       </c>
@@ -6231,9 +6243,9 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" s="26"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="50"/>
+      <c r="A73" s="50"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="28"/>
       <c r="D73" s="6" t="s">
         <v>327</v>
       </c>
@@ -6253,9 +6265,9 @@
       <c r="J73" s="15"/>
     </row>
     <row r="74" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="26"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="50"/>
+      <c r="A74" s="50"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="28"/>
       <c r="D74" s="6" t="s">
         <v>328</v>
       </c>
@@ -6277,9 +6289,9 @@
       <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="26"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="51"/>
+      <c r="A75" s="50"/>
+      <c r="B75" s="50"/>
+      <c r="C75" s="29"/>
       <c r="D75" s="6" t="s">
         <v>330</v>
       </c>
@@ -6299,13 +6311,13 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="25" t="s">
+      <c r="A76" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="C76" s="38" t="s">
+      <c r="C76" s="30" t="s">
         <v>785</v>
       </c>
       <c r="D76" s="2" t="s">
@@ -6329,9 +6341,9 @@
       <c r="J76" s="16"/>
     </row>
     <row r="77" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="40"/>
+      <c r="A77" s="54"/>
+      <c r="B77" s="54"/>
+      <c r="C77" s="31"/>
       <c r="D77" s="2" t="s">
         <v>59</v>
       </c>
@@ -6353,9 +6365,9 @@
       <c r="J77" s="16"/>
     </row>
     <row r="78" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="25"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="40"/>
+      <c r="A78" s="54"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="31"/>
       <c r="D78" s="2" t="s">
         <v>290</v>
       </c>
@@ -6375,9 +6387,9 @@
       <c r="J78" s="16"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="40"/>
+      <c r="A79" s="54"/>
+      <c r="B79" s="54"/>
+      <c r="C79" s="31"/>
       <c r="D79" s="2" t="s">
         <v>60</v>
       </c>
@@ -6397,9 +6409,9 @@
       <c r="J79" s="16"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" s="25"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="39"/>
+      <c r="A80" s="54"/>
+      <c r="B80" s="54"/>
+      <c r="C80" s="32"/>
       <c r="D80" s="2" t="s">
         <v>284</v>
       </c>
@@ -6419,13 +6431,13 @@
       <c r="J80" s="16"/>
     </row>
     <row r="81" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A81" s="24" t="s">
+      <c r="A81" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B81" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C81" s="27" t="s">
+      <c r="C81" s="33" t="s">
         <v>786</v>
       </c>
       <c r="D81" s="3" t="s">
@@ -6449,9 +6461,9 @@
       <c r="J81" s="18"/>
     </row>
     <row r="82" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="24"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="28"/>
+      <c r="A82" s="55"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="34"/>
       <c r="D82" s="3" t="s">
         <v>64</v>
       </c>
@@ -6473,9 +6485,9 @@
       <c r="J82" s="18"/>
     </row>
     <row r="83" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A83" s="24"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="28"/>
+      <c r="A83" s="55"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="34"/>
       <c r="D83" s="3" t="s">
         <v>300</v>
       </c>
@@ -6495,9 +6507,9 @@
       <c r="J83" s="18"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="28"/>
+      <c r="A84" s="55"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="34"/>
       <c r="D84" s="3" t="s">
         <v>65</v>
       </c>
@@ -6517,9 +6529,9 @@
       <c r="J84" s="18"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="24"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="29"/>
+      <c r="A85" s="55"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="35"/>
       <c r="D85" s="3" t="s">
         <v>848</v>
       </c>
@@ -6539,13 +6551,13 @@
       <c r="J85" s="18"/>
     </row>
     <row r="86" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A86" s="30" t="s">
+      <c r="A86" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B86" s="30" t="s">
+      <c r="B86" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C86" s="32" t="s">
+      <c r="C86" s="38" t="s">
         <v>787</v>
       </c>
       <c r="D86" s="4" t="s">
@@ -6569,9 +6581,9 @@
       <c r="J86" s="14"/>
     </row>
     <row r="87" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="33"/>
+      <c r="A87" s="46"/>
+      <c r="B87" s="46"/>
+      <c r="C87" s="39"/>
       <c r="D87" s="4" t="s">
         <v>73</v>
       </c>
@@ -6591,9 +6603,9 @@
       <c r="J87" s="14"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="34"/>
+      <c r="A88" s="46"/>
+      <c r="B88" s="46"/>
+      <c r="C88" s="40"/>
       <c r="D88" s="4" t="s">
         <v>74</v>
       </c>
@@ -6613,61 +6625,61 @@
       <c r="J88" s="14"/>
     </row>
     <row r="89" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30"/>
-      <c r="C89" s="56" t="s">
+      <c r="A89" s="46"/>
+      <c r="B89" s="46"/>
+      <c r="C89" s="47" t="s">
         <v>788</v>
       </c>
-      <c r="D89" s="55" t="s">
+      <c r="D89" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="E89" s="55" t="s">
+      <c r="E89" s="24" t="s">
         <v>353</v>
       </c>
-      <c r="F89" s="55" t="s">
+      <c r="F89" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="G89" s="55" t="s">
+      <c r="G89" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="H89" s="54">
+      <c r="H89" s="23">
         <v>4</v>
       </c>
-      <c r="I89" s="54" t="s">
+      <c r="I89" s="23" t="s">
         <v>717</v>
       </c>
-      <c r="J89" s="54"/>
+      <c r="J89" s="23"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="55" t="s">
+      <c r="A90" s="46"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="48"/>
+      <c r="D90" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="E90" s="55" t="s">
+      <c r="E90" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="F90" s="55" t="s">
+      <c r="F90" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="G90" s="55"/>
-      <c r="H90" s="54">
+      <c r="G90" s="24"/>
+      <c r="H90" s="23">
         <v>4</v>
       </c>
-      <c r="I90" s="54" t="s">
+      <c r="I90" s="23" t="s">
         <v>717</v>
       </c>
-      <c r="J90" s="54"/>
+      <c r="J90" s="23"/>
     </row>
     <row r="91" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A91" s="31" t="s">
+      <c r="A91" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="C91" s="35" t="s">
+      <c r="C91" s="43" t="s">
         <v>789</v>
       </c>
       <c r="D91" s="5" t="s">
@@ -6691,9 +6703,9 @@
       <c r="J91" s="17"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="31"/>
-      <c r="B92" s="31"/>
-      <c r="C92" s="37"/>
+      <c r="A92" s="52"/>
+      <c r="B92" s="52"/>
+      <c r="C92" s="45"/>
       <c r="D92" s="5" t="s">
         <v>77</v>
       </c>
@@ -6713,13 +6725,13 @@
       <c r="J92" s="17"/>
     </row>
     <row r="93" spans="1:10" ht="165" x14ac:dyDescent="0.3">
-      <c r="A93" s="26" t="s">
+      <c r="A93" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B93" s="26" t="s">
+      <c r="B93" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C93" s="49" t="s">
+      <c r="C93" s="27" t="s">
         <v>790</v>
       </c>
       <c r="D93" s="6" t="s">
@@ -6745,9 +6757,9 @@
       </c>
     </row>
     <row r="94" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A94" s="26"/>
-      <c r="B94" s="26"/>
-      <c r="C94" s="50"/>
+      <c r="A94" s="50"/>
+      <c r="B94" s="50"/>
+      <c r="C94" s="28"/>
       <c r="D94" s="6" t="s">
         <v>89</v>
       </c>
@@ -6769,9 +6781,9 @@
       <c r="J94" s="15"/>
     </row>
     <row r="95" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="50"/>
+      <c r="A95" s="50"/>
+      <c r="B95" s="50"/>
+      <c r="C95" s="28"/>
       <c r="D95" s="6" t="s">
         <v>90</v>
       </c>
@@ -6791,9 +6803,9 @@
       <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="50"/>
+      <c r="A96" s="50"/>
+      <c r="B96" s="50"/>
+      <c r="C96" s="28"/>
       <c r="D96" s="6" t="s">
         <v>414</v>
       </c>
@@ -6813,13 +6825,13 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="B97" s="25" t="s">
+      <c r="B97" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="C97" s="38" t="s">
+      <c r="C97" s="30" t="s">
         <v>792</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -6843,9 +6855,9 @@
       <c r="J97" s="16"/>
     </row>
     <row r="98" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A98" s="25"/>
-      <c r="B98" s="25"/>
-      <c r="C98" s="40"/>
+      <c r="A98" s="54"/>
+      <c r="B98" s="54"/>
+      <c r="C98" s="31"/>
       <c r="D98" s="2" t="s">
         <v>455</v>
       </c>
@@ -6869,9 +6881,9 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A99" s="25"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="40"/>
+      <c r="A99" s="54"/>
+      <c r="B99" s="54"/>
+      <c r="C99" s="31"/>
       <c r="D99" s="2" t="s">
         <v>107</v>
       </c>
@@ -6891,9 +6903,9 @@
       <c r="J99" s="16"/>
     </row>
     <row r="100" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A100" s="25"/>
-      <c r="B100" s="25"/>
-      <c r="C100" s="40"/>
+      <c r="A100" s="54"/>
+      <c r="B100" s="54"/>
+      <c r="C100" s="31"/>
       <c r="D100" s="2" t="s">
         <v>463</v>
       </c>
@@ -6913,9 +6925,9 @@
       <c r="J100" s="16"/>
     </row>
     <row r="101" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A101" s="25"/>
-      <c r="B101" s="25"/>
-      <c r="C101" s="40"/>
+      <c r="A101" s="54"/>
+      <c r="B101" s="54"/>
+      <c r="C101" s="31"/>
       <c r="D101" s="2" t="s">
         <v>108</v>
       </c>
@@ -6935,9 +6947,9 @@
       <c r="J101" s="16"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A102" s="25"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="39"/>
+      <c r="A102" s="54"/>
+      <c r="B102" s="54"/>
+      <c r="C102" s="32"/>
       <c r="D102" s="2" t="s">
         <v>462</v>
       </c>
@@ -6947,23 +6959,23 @@
       <c r="F102" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="G102" s="60"/>
+      <c r="G102" s="25"/>
       <c r="H102" s="16">
         <v>4</v>
       </c>
-      <c r="I102" s="61" t="s">
+      <c r="I102" s="26" t="s">
         <v>719</v>
       </c>
-      <c r="J102" s="61"/>
+      <c r="J102" s="26"/>
     </row>
     <row r="103" spans="1:10" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="24" t="s">
+      <c r="A103" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="27" t="s">
+      <c r="C103" s="33" t="s">
         <v>791</v>
       </c>
       <c r="D103" s="3" t="s">
@@ -6984,14 +6996,14 @@
       <c r="I103" s="18" t="s">
         <v>719</v>
       </c>
-      <c r="J103" s="27" t="s">
+      <c r="J103" s="33" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A104" s="24"/>
-      <c r="B104" s="24"/>
-      <c r="C104" s="29"/>
+      <c r="A104" s="55"/>
+      <c r="B104" s="55"/>
+      <c r="C104" s="35"/>
       <c r="D104" s="3" t="s">
         <v>104</v>
       </c>
@@ -7008,16 +7020,16 @@
       <c r="I104" s="18" t="s">
         <v>719</v>
       </c>
-      <c r="J104" s="29"/>
+      <c r="J104" s="35"/>
     </row>
     <row r="105" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A105" s="30" t="s">
+      <c r="A105" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B105" s="30" t="s">
+      <c r="B105" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C105" s="32" t="s">
+      <c r="C105" s="38" t="s">
         <v>793</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -7041,9 +7053,9 @@
       <c r="J105" s="14"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="30"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="33"/>
+      <c r="A106" s="46"/>
+      <c r="B106" s="46"/>
+      <c r="C106" s="39"/>
       <c r="D106" s="4" t="s">
         <v>33</v>
       </c>
@@ -7063,9 +7075,9 @@
       <c r="J106" s="14"/>
     </row>
     <row r="107" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="30"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="33"/>
+      <c r="A107" s="46"/>
+      <c r="B107" s="46"/>
+      <c r="C107" s="39"/>
       <c r="D107" s="4" t="s">
         <v>453</v>
       </c>
@@ -7085,9 +7097,9 @@
       <c r="J107" s="14"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A108" s="30"/>
-      <c r="B108" s="30"/>
-      <c r="C108" s="33"/>
+      <c r="A108" s="46"/>
+      <c r="B108" s="46"/>
+      <c r="C108" s="39"/>
       <c r="D108" s="4" t="s">
         <v>34</v>
       </c>
@@ -7107,61 +7119,61 @@
       <c r="J108" s="14"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A109" s="30"/>
-      <c r="B109" s="30"/>
-      <c r="C109" s="34"/>
-      <c r="D109" s="4" t="s">
+      <c r="A109" s="46"/>
+      <c r="B109" s="46"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="62" t="s">
         <v>427</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="62" t="s">
         <v>428</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="F109" s="62" t="s">
         <v>429</v>
       </c>
-      <c r="G109" s="4"/>
-      <c r="H109" s="14">
+      <c r="G109" s="62"/>
+      <c r="H109" s="63">
         <v>3</v>
       </c>
-      <c r="I109" s="14" t="s">
-        <v>474</v>
-      </c>
-      <c r="J109" s="14"/>
+      <c r="I109" s="63" t="s">
+        <v>474</v>
+      </c>
+      <c r="J109" s="63"/>
     </row>
     <row r="110" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A110" s="30"/>
-      <c r="B110" s="30"/>
-      <c r="C110" s="54" t="s">
+      <c r="A110" s="46"/>
+      <c r="B110" s="46"/>
+      <c r="C110" s="23" t="s">
         <v>794</v>
       </c>
-      <c r="D110" s="55" t="s">
+      <c r="D110" s="24" t="s">
         <v>477</v>
       </c>
-      <c r="E110" s="55" t="s">
+      <c r="E110" s="24" t="s">
         <v>478</v>
       </c>
-      <c r="F110" s="55" t="s">
+      <c r="F110" s="24" t="s">
         <v>489</v>
       </c>
-      <c r="G110" s="55" t="s">
+      <c r="G110" s="24" t="s">
         <v>488</v>
       </c>
-      <c r="H110" s="54">
+      <c r="H110" s="23">
         <v>3</v>
       </c>
-      <c r="I110" s="54" t="s">
-        <v>474</v>
-      </c>
-      <c r="J110" s="54"/>
+      <c r="I110" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="J110" s="23"/>
     </row>
     <row r="111" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A111" s="31" t="s">
+      <c r="A111" s="52" t="s">
         <v>448</v>
       </c>
-      <c r="B111" s="31" t="s">
+      <c r="B111" s="52" t="s">
         <v>447</v>
       </c>
-      <c r="C111" s="35" t="s">
+      <c r="C111" s="43" t="s">
         <v>795</v>
       </c>
       <c r="D111" s="5" t="s">
@@ -7185,9 +7197,9 @@
       <c r="J111" s="17"/>
     </row>
     <row r="112" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A112" s="31"/>
-      <c r="B112" s="31"/>
-      <c r="C112" s="37"/>
+      <c r="A112" s="52"/>
+      <c r="B112" s="52"/>
+      <c r="C112" s="45"/>
       <c r="D112" s="5" t="s">
         <v>450</v>
       </c>
@@ -7207,85 +7219,85 @@
       <c r="J112" s="17"/>
     </row>
     <row r="113" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A113" s="31"/>
-      <c r="B113" s="31"/>
-      <c r="C113" s="45" t="s">
+      <c r="A113" s="52"/>
+      <c r="B113" s="52"/>
+      <c r="C113" s="41" t="s">
         <v>796</v>
       </c>
-      <c r="D113" s="46" t="s">
+      <c r="D113" s="21" t="s">
         <v>495</v>
       </c>
-      <c r="E113" s="46" t="s">
+      <c r="E113" s="21" t="s">
         <v>497</v>
       </c>
-      <c r="F113" s="46" t="s">
+      <c r="F113" s="21" t="s">
         <v>498</v>
       </c>
-      <c r="G113" s="46" t="s">
+      <c r="G113" s="21" t="s">
         <v>501</v>
       </c>
-      <c r="H113" s="47">
+      <c r="H113" s="22">
         <v>2</v>
       </c>
-      <c r="I113" s="47" t="s">
-        <v>474</v>
-      </c>
-      <c r="J113" s="47"/>
+      <c r="I113" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="J113" s="22"/>
     </row>
     <row r="114" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A114" s="31"/>
-      <c r="B114" s="31"/>
-      <c r="C114" s="58"/>
-      <c r="D114" s="46" t="s">
+      <c r="A114" s="52"/>
+      <c r="B114" s="52"/>
+      <c r="C114" s="49"/>
+      <c r="D114" s="21" t="s">
         <v>496</v>
       </c>
-      <c r="E114" s="46" t="s">
+      <c r="E114" s="21" t="s">
         <v>492</v>
       </c>
-      <c r="F114" s="46" t="s">
+      <c r="F114" s="21" t="s">
         <v>503</v>
       </c>
-      <c r="G114" s="46" t="s">
+      <c r="G114" s="21" t="s">
         <v>504</v>
       </c>
-      <c r="H114" s="47">
+      <c r="H114" s="22">
         <v>2</v>
       </c>
-      <c r="I114" s="47" t="s">
-        <v>474</v>
-      </c>
-      <c r="J114" s="47"/>
+      <c r="I114" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="J114" s="22"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A115" s="31"/>
-      <c r="B115" s="31"/>
-      <c r="C115" s="48"/>
-      <c r="D115" s="46" t="s">
+      <c r="A115" s="52"/>
+      <c r="B115" s="52"/>
+      <c r="C115" s="42"/>
+      <c r="D115" s="21" t="s">
         <v>499</v>
       </c>
-      <c r="E115" s="46" t="s">
+      <c r="E115" s="21" t="s">
         <v>500</v>
       </c>
-      <c r="F115" s="46" t="s">
+      <c r="F115" s="21" t="s">
         <v>505</v>
       </c>
-      <c r="G115" s="46"/>
-      <c r="H115" s="47">
+      <c r="G115" s="21"/>
+      <c r="H115" s="22">
         <v>2</v>
       </c>
-      <c r="I115" s="47" t="s">
-        <v>474</v>
-      </c>
-      <c r="J115" s="47"/>
+      <c r="I115" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="J115" s="22"/>
     </row>
     <row r="116" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A116" s="26" t="s">
+      <c r="A116" s="50" t="s">
         <v>493</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="B116" s="50" t="s">
         <v>512</v>
       </c>
-      <c r="C116" s="49" t="s">
+      <c r="C116" s="27" t="s">
         <v>797</v>
       </c>
       <c r="D116" s="6" t="s">
@@ -7309,9 +7321,9 @@
       <c r="J116" s="15"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A117" s="26"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="50"/>
+      <c r="A117" s="50"/>
+      <c r="B117" s="50"/>
+      <c r="C117" s="28"/>
       <c r="D117" s="6" t="s">
         <v>507</v>
       </c>
@@ -7331,9 +7343,9 @@
       <c r="J117" s="15"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A118" s="26"/>
-      <c r="B118" s="26"/>
-      <c r="C118" s="51"/>
+      <c r="A118" s="50"/>
+      <c r="B118" s="50"/>
+      <c r="C118" s="29"/>
       <c r="D118" s="6" t="s">
         <v>518</v>
       </c>
@@ -7353,13 +7365,13 @@
       <c r="J118" s="15"/>
     </row>
     <row r="119" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A119" s="25" t="s">
+      <c r="A119" s="54" t="s">
         <v>508</v>
       </c>
-      <c r="B119" s="25" t="s">
+      <c r="B119" s="54" t="s">
         <v>494</v>
       </c>
-      <c r="C119" s="38" t="s">
+      <c r="C119" s="30" t="s">
         <v>798</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -7383,9 +7395,9 @@
       <c r="J119" s="16"/>
     </row>
     <row r="120" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A120" s="25"/>
-      <c r="B120" s="25"/>
-      <c r="C120" s="40"/>
+      <c r="A120" s="54"/>
+      <c r="B120" s="54"/>
+      <c r="C120" s="31"/>
       <c r="D120" s="2" t="s">
         <v>510</v>
       </c>
@@ -7407,9 +7419,9 @@
       <c r="J120" s="16"/>
     </row>
     <row r="121" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A121" s="25"/>
-      <c r="B121" s="25"/>
-      <c r="C121" s="40"/>
+      <c r="A121" s="54"/>
+      <c r="B121" s="54"/>
+      <c r="C121" s="31"/>
       <c r="D121" s="2" t="s">
         <v>524</v>
       </c>
@@ -7431,9 +7443,9 @@
       <c r="J121" s="16"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A122" s="25"/>
-      <c r="B122" s="25"/>
-      <c r="C122" s="40"/>
+      <c r="A122" s="54"/>
+      <c r="B122" s="54"/>
+      <c r="C122" s="31"/>
       <c r="D122" s="2" t="s">
         <v>511</v>
       </c>
@@ -7453,9 +7465,9 @@
       <c r="J122" s="16"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A123" s="25"/>
-      <c r="B123" s="25"/>
-      <c r="C123" s="40"/>
+      <c r="A123" s="54"/>
+      <c r="B123" s="54"/>
+      <c r="C123" s="31"/>
       <c r="D123" s="2" t="s">
         <v>530</v>
       </c>
@@ -7477,13 +7489,13 @@
       <c r="J123" s="16"/>
     </row>
     <row r="124" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A124" s="24" t="s">
+      <c r="A124" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B124" s="24" t="s">
+      <c r="B124" s="55" t="s">
         <v>537</v>
       </c>
-      <c r="C124" s="27" t="s">
+      <c r="C124" s="33" t="s">
         <v>799</v>
       </c>
       <c r="D124" s="3" t="s">
@@ -7507,9 +7519,9 @@
       <c r="J124" s="18"/>
     </row>
     <row r="125" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A125" s="24"/>
-      <c r="B125" s="24"/>
-      <c r="C125" s="28"/>
+      <c r="A125" s="55"/>
+      <c r="B125" s="55"/>
+      <c r="C125" s="34"/>
       <c r="D125" s="3" t="s">
         <v>544</v>
       </c>
@@ -7529,9 +7541,9 @@
       <c r="J125" s="18"/>
     </row>
     <row r="126" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A126" s="24"/>
-      <c r="B126" s="24"/>
-      <c r="C126" s="28"/>
+      <c r="A126" s="55"/>
+      <c r="B126" s="55"/>
+      <c r="C126" s="34"/>
       <c r="D126" s="3" t="s">
         <v>543</v>
       </c>
@@ -7553,9 +7565,9 @@
       <c r="J126" s="18"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A127" s="24"/>
-      <c r="B127" s="24"/>
-      <c r="C127" s="29"/>
+      <c r="A127" s="55"/>
+      <c r="B127" s="55"/>
+      <c r="C127" s="35"/>
       <c r="D127" s="3" t="s">
         <v>38</v>
       </c>
@@ -7575,13 +7587,13 @@
       <c r="J127" s="18"/>
     </row>
     <row r="128" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A128" s="30" t="s">
+      <c r="A128" s="46" t="s">
         <v>563</v>
       </c>
-      <c r="B128" s="30" t="s">
+      <c r="B128" s="46" t="s">
         <v>564</v>
       </c>
-      <c r="C128" s="32" t="s">
+      <c r="C128" s="38" t="s">
         <v>796</v>
       </c>
       <c r="D128" s="4" t="s">
@@ -7605,9 +7617,9 @@
       <c r="J128" s="14"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A129" s="30"/>
-      <c r="B129" s="30"/>
-      <c r="C129" s="33"/>
+      <c r="A129" s="46"/>
+      <c r="B129" s="46"/>
+      <c r="C129" s="39"/>
       <c r="D129" s="4" t="s">
         <v>550</v>
       </c>
@@ -7629,9 +7641,9 @@
       <c r="J129" s="14"/>
     </row>
     <row r="130" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A130" s="30"/>
-      <c r="B130" s="30"/>
-      <c r="C130" s="33"/>
+      <c r="A130" s="46"/>
+      <c r="B130" s="46"/>
+      <c r="C130" s="39"/>
       <c r="D130" s="4" t="s">
         <v>566</v>
       </c>
@@ -7653,9 +7665,9 @@
       <c r="J130" s="14"/>
     </row>
     <row r="131" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A131" s="30"/>
-      <c r="B131" s="30"/>
-      <c r="C131" s="33"/>
+      <c r="A131" s="46"/>
+      <c r="B131" s="46"/>
+      <c r="C131" s="39"/>
       <c r="D131" s="12" t="s">
         <v>557</v>
       </c>
@@ -7677,9 +7689,9 @@
       <c r="J131" s="14"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A132" s="30"/>
-      <c r="B132" s="30"/>
-      <c r="C132" s="34"/>
+      <c r="A132" s="46"/>
+      <c r="B132" s="46"/>
+      <c r="C132" s="40"/>
       <c r="D132" s="4" t="s">
         <v>555</v>
       </c>
@@ -7699,13 +7711,13 @@
       <c r="J132" s="14"/>
     </row>
     <row r="133" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A133" s="31" t="s">
+      <c r="A133" s="52" t="s">
         <v>559</v>
       </c>
-      <c r="B133" s="31" t="s">
+      <c r="B133" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C133" s="35" t="s">
+      <c r="C133" s="43" t="s">
         <v>800</v>
       </c>
       <c r="D133" s="5" t="s">
@@ -7731,9 +7743,9 @@
       </c>
     </row>
     <row r="134" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A134" s="31"/>
-      <c r="B134" s="31"/>
-      <c r="C134" s="36"/>
+      <c r="A134" s="52"/>
+      <c r="B134" s="52"/>
+      <c r="C134" s="44"/>
       <c r="D134" s="5" t="s">
         <v>556</v>
       </c>
@@ -7755,9 +7767,9 @@
       <c r="J134" s="17"/>
     </row>
     <row r="135" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A135" s="31"/>
-      <c r="B135" s="31"/>
-      <c r="C135" s="36"/>
+      <c r="A135" s="52"/>
+      <c r="B135" s="52"/>
+      <c r="C135" s="44"/>
       <c r="D135" s="5" t="s">
         <v>561</v>
       </c>
@@ -7779,9 +7791,9 @@
       <c r="J135" s="17"/>
     </row>
     <row r="136" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A136" s="31"/>
-      <c r="B136" s="31"/>
-      <c r="C136" s="37"/>
+      <c r="A136" s="52"/>
+      <c r="B136" s="52"/>
+      <c r="C136" s="45"/>
       <c r="D136" s="5" t="s">
         <v>562</v>
       </c>
@@ -7801,13 +7813,13 @@
       <c r="J136" s="17"/>
     </row>
     <row r="137" spans="1:10" ht="99" x14ac:dyDescent="0.3">
-      <c r="A137" s="26" t="s">
+      <c r="A137" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B137" s="26" t="s">
+      <c r="B137" s="50" t="s">
         <v>346</v>
       </c>
-      <c r="C137" s="49" t="s">
+      <c r="C137" s="27" t="s">
         <v>801</v>
       </c>
       <c r="D137" s="6" t="s">
@@ -7831,9 +7843,9 @@
       <c r="J137" s="15"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A138" s="26"/>
-      <c r="B138" s="26"/>
-      <c r="C138" s="50"/>
+      <c r="A138" s="50"/>
+      <c r="B138" s="50"/>
+      <c r="C138" s="28"/>
       <c r="D138" s="6" t="s">
         <v>589</v>
       </c>
@@ -7853,9 +7865,9 @@
       <c r="J138" s="15"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A139" s="26"/>
-      <c r="B139" s="26"/>
-      <c r="C139" s="50"/>
+      <c r="A139" s="50"/>
+      <c r="B139" s="50"/>
+      <c r="C139" s="28"/>
       <c r="D139" s="6" t="s">
         <v>590</v>
       </c>
@@ -7875,9 +7887,9 @@
       <c r="J139" s="15"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A140" s="26"/>
-      <c r="B140" s="26"/>
-      <c r="C140" s="50"/>
+      <c r="A140" s="50"/>
+      <c r="B140" s="50"/>
+      <c r="C140" s="28"/>
       <c r="D140" s="6" t="s">
         <v>591</v>
       </c>
@@ -7897,9 +7909,9 @@
       <c r="J140" s="15"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A141" s="26"/>
-      <c r="B141" s="26"/>
-      <c r="C141" s="51"/>
+      <c r="A141" s="50"/>
+      <c r="B141" s="50"/>
+      <c r="C141" s="29"/>
       <c r="D141" s="6" t="s">
         <v>594</v>
       </c>
@@ -7919,13 +7931,13 @@
       <c r="J141" s="15"/>
     </row>
     <row r="142" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A142" s="25" t="s">
+      <c r="A142" s="54" t="s">
         <v>824</v>
       </c>
-      <c r="B142" s="25" t="s">
+      <c r="B142" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="C142" s="38" t="s">
+      <c r="C142" s="30" t="s">
         <v>803</v>
       </c>
       <c r="D142" s="2" t="s">
@@ -7949,9 +7961,9 @@
       <c r="J142" s="16"/>
     </row>
     <row r="143" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A143" s="25"/>
-      <c r="B143" s="25"/>
-      <c r="C143" s="40"/>
+      <c r="A143" s="54"/>
+      <c r="B143" s="54"/>
+      <c r="C143" s="31"/>
       <c r="D143" s="2" t="s">
         <v>605</v>
       </c>
@@ -7973,9 +7985,9 @@
       <c r="J143" s="16"/>
     </row>
     <row r="144" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A144" s="25"/>
-      <c r="B144" s="25"/>
-      <c r="C144" s="40"/>
+      <c r="A144" s="54"/>
+      <c r="B144" s="54"/>
+      <c r="C144" s="31"/>
       <c r="D144" s="2" t="s">
         <v>611</v>
       </c>
@@ -7995,9 +8007,9 @@
       <c r="J144" s="16"/>
     </row>
     <row r="145" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A145" s="25"/>
-      <c r="B145" s="25"/>
-      <c r="C145" s="40"/>
+      <c r="A145" s="54"/>
+      <c r="B145" s="54"/>
+      <c r="C145" s="31"/>
       <c r="D145" s="2" t="s">
         <v>610</v>
       </c>
@@ -8019,9 +8031,9 @@
       <c r="J145" s="16"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A146" s="25"/>
-      <c r="B146" s="25"/>
-      <c r="C146" s="40"/>
+      <c r="A146" s="54"/>
+      <c r="B146" s="54"/>
+      <c r="C146" s="31"/>
       <c r="D146" s="2" t="s">
         <v>43</v>
       </c>
@@ -8041,9 +8053,9 @@
       <c r="J146" s="16"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A147" s="25"/>
-      <c r="B147" s="25"/>
-      <c r="C147" s="40"/>
+      <c r="A147" s="54"/>
+      <c r="B147" s="54"/>
+      <c r="C147" s="31"/>
       <c r="D147" s="2" t="s">
         <v>604</v>
       </c>
@@ -8063,9 +8075,9 @@
       <c r="J147" s="16"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A148" s="25"/>
-      <c r="B148" s="25"/>
-      <c r="C148" s="40"/>
+      <c r="A148" s="54"/>
+      <c r="B148" s="54"/>
+      <c r="C148" s="31"/>
       <c r="D148" s="2" t="s">
         <v>603</v>
       </c>
@@ -8085,13 +8097,13 @@
       <c r="J148" s="16"/>
     </row>
     <row r="149" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A149" s="24" t="s">
+      <c r="A149" s="55" t="s">
         <v>825</v>
       </c>
-      <c r="B149" s="24" t="s">
+      <c r="B149" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="C149" s="27" t="s">
+      <c r="C149" s="33" t="s">
         <v>805</v>
       </c>
       <c r="D149" s="3" t="s">
@@ -8115,9 +8127,9 @@
       <c r="J149" s="18"/>
     </row>
     <row r="150" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A150" s="24"/>
-      <c r="B150" s="24"/>
-      <c r="C150" s="28"/>
+      <c r="A150" s="55"/>
+      <c r="B150" s="55"/>
+      <c r="C150" s="34"/>
       <c r="D150" s="3" t="s">
         <v>616</v>
       </c>
@@ -8139,9 +8151,9 @@
       <c r="J150" s="18"/>
     </row>
     <row r="151" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A151" s="24"/>
-      <c r="B151" s="24"/>
-      <c r="C151" s="28"/>
+      <c r="A151" s="55"/>
+      <c r="B151" s="55"/>
+      <c r="C151" s="34"/>
       <c r="D151" s="3" t="s">
         <v>617</v>
       </c>
@@ -8161,9 +8173,9 @@
       <c r="J151" s="18"/>
     </row>
     <row r="152" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A152" s="24"/>
-      <c r="B152" s="24"/>
-      <c r="C152" s="28"/>
+      <c r="A152" s="55"/>
+      <c r="B152" s="55"/>
+      <c r="C152" s="34"/>
       <c r="D152" s="3" t="s">
         <v>618</v>
       </c>
@@ -8185,9 +8197,9 @@
       <c r="J152" s="18"/>
     </row>
     <row r="153" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A153" s="24"/>
-      <c r="B153" s="24"/>
-      <c r="C153" s="28"/>
+      <c r="A153" s="55"/>
+      <c r="B153" s="55"/>
+      <c r="C153" s="34"/>
       <c r="D153" s="3" t="s">
         <v>838</v>
       </c>
@@ -8207,9 +8219,9 @@
       <c r="J153" s="18"/>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A154" s="24"/>
-      <c r="B154" s="24"/>
-      <c r="C154" s="28"/>
+      <c r="A154" s="55"/>
+      <c r="B154" s="55"/>
+      <c r="C154" s="34"/>
       <c r="D154" s="3" t="s">
         <v>839</v>
       </c>
@@ -8229,9 +8241,9 @@
       <c r="J154" s="18"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A155" s="24"/>
-      <c r="B155" s="24"/>
-      <c r="C155" s="28"/>
+      <c r="A155" s="55"/>
+      <c r="B155" s="55"/>
+      <c r="C155" s="34"/>
       <c r="D155" s="3" t="s">
         <v>840</v>
       </c>
@@ -8251,13 +8263,13 @@
       <c r="J155" s="18"/>
     </row>
     <row r="156" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A156" s="30" t="s">
+      <c r="A156" s="46" t="s">
         <v>826</v>
       </c>
-      <c r="B156" s="30" t="s">
+      <c r="B156" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="C156" s="32" t="s">
+      <c r="C156" s="38" t="s">
         <v>804</v>
       </c>
       <c r="D156" s="4" t="s">
@@ -8281,9 +8293,9 @@
       <c r="J156" s="14"/>
     </row>
     <row r="157" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A157" s="30"/>
-      <c r="B157" s="30"/>
-      <c r="C157" s="33"/>
+      <c r="A157" s="46"/>
+      <c r="B157" s="46"/>
+      <c r="C157" s="39"/>
       <c r="D157" s="4" t="s">
         <v>842</v>
       </c>
@@ -8305,9 +8317,9 @@
       <c r="J157" s="14"/>
     </row>
     <row r="158" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A158" s="30"/>
-      <c r="B158" s="30"/>
-      <c r="C158" s="33"/>
+      <c r="A158" s="46"/>
+      <c r="B158" s="46"/>
+      <c r="C158" s="39"/>
       <c r="D158" s="4" t="s">
         <v>843</v>
       </c>
@@ -8327,9 +8339,9 @@
       <c r="J158" s="14"/>
     </row>
     <row r="159" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A159" s="30"/>
-      <c r="B159" s="30"/>
-      <c r="C159" s="33"/>
+      <c r="A159" s="46"/>
+      <c r="B159" s="46"/>
+      <c r="C159" s="39"/>
       <c r="D159" s="4" t="s">
         <v>844</v>
       </c>
@@ -8351,9 +8363,9 @@
       <c r="J159" s="14"/>
     </row>
     <row r="160" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A160" s="30"/>
-      <c r="B160" s="30"/>
-      <c r="C160" s="33"/>
+      <c r="A160" s="46"/>
+      <c r="B160" s="46"/>
+      <c r="C160" s="39"/>
       <c r="D160" s="4" t="s">
         <v>845</v>
       </c>
@@ -8373,9 +8385,9 @@
       <c r="J160" s="14"/>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A161" s="30"/>
-      <c r="B161" s="30"/>
-      <c r="C161" s="33"/>
+      <c r="A161" s="46"/>
+      <c r="B161" s="46"/>
+      <c r="C161" s="39"/>
       <c r="D161" s="4" t="s">
         <v>846</v>
       </c>
@@ -8395,9 +8407,9 @@
       <c r="J161" s="14"/>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A162" s="30"/>
-      <c r="B162" s="30"/>
-      <c r="C162" s="34"/>
+      <c r="A162" s="46"/>
+      <c r="B162" s="46"/>
+      <c r="C162" s="40"/>
       <c r="D162" s="4" t="s">
         <v>847</v>
       </c>
@@ -8417,13 +8429,13 @@
       <c r="J162" s="14"/>
     </row>
     <row r="163" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A163" s="31" t="s">
+      <c r="A163" s="52" t="s">
         <v>651</v>
       </c>
-      <c r="B163" s="31" t="s">
+      <c r="B163" s="52" t="s">
         <v>652</v>
       </c>
-      <c r="C163" s="35" t="s">
+      <c r="C163" s="43" t="s">
         <v>806</v>
       </c>
       <c r="D163" s="5" t="s">
@@ -8447,9 +8459,9 @@
       <c r="J163" s="17"/>
     </row>
     <row r="164" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A164" s="31"/>
-      <c r="B164" s="31"/>
-      <c r="C164" s="36"/>
+      <c r="A164" s="52"/>
+      <c r="B164" s="52"/>
+      <c r="C164" s="44"/>
       <c r="D164" s="5" t="s">
         <v>242</v>
       </c>
@@ -8471,9 +8483,9 @@
       <c r="J164" s="17"/>
     </row>
     <row r="165" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A165" s="31"/>
-      <c r="B165" s="31"/>
-      <c r="C165" s="36"/>
+      <c r="A165" s="52"/>
+      <c r="B165" s="52"/>
+      <c r="C165" s="44"/>
       <c r="D165" s="5" t="s">
         <v>657</v>
       </c>
@@ -8495,9 +8507,9 @@
       <c r="J165" s="17"/>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A166" s="31"/>
-      <c r="B166" s="31"/>
-      <c r="C166" s="37"/>
+      <c r="A166" s="52"/>
+      <c r="B166" s="52"/>
+      <c r="C166" s="45"/>
       <c r="D166" s="5" t="s">
         <v>243</v>
       </c>
@@ -8517,13 +8529,13 @@
       <c r="J166" s="17"/>
     </row>
     <row r="167" spans="1:10" ht="165" x14ac:dyDescent="0.3">
-      <c r="A167" s="26" t="s">
+      <c r="A167" s="50" t="s">
         <v>645</v>
       </c>
-      <c r="B167" s="26" t="s">
+      <c r="B167" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C167" s="49" t="s">
+      <c r="C167" s="27" t="s">
         <v>807</v>
       </c>
       <c r="D167" s="6" t="s">
@@ -8547,9 +8559,9 @@
       <c r="J167" s="15"/>
     </row>
     <row r="168" spans="1:10" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A168" s="26"/>
-      <c r="B168" s="26"/>
-      <c r="C168" s="50"/>
+      <c r="A168" s="50"/>
+      <c r="B168" s="50"/>
+      <c r="C168" s="28"/>
       <c r="D168" s="6" t="s">
         <v>668</v>
       </c>
@@ -8571,9 +8583,9 @@
       <c r="J168" s="15"/>
     </row>
     <row r="169" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A169" s="26"/>
-      <c r="B169" s="26"/>
-      <c r="C169" s="50"/>
+      <c r="A169" s="50"/>
+      <c r="B169" s="50"/>
+      <c r="C169" s="28"/>
       <c r="D169" s="6" t="s">
         <v>667</v>
       </c>
@@ -8595,9 +8607,9 @@
       <c r="J169" s="15"/>
     </row>
     <row r="170" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A170" s="26"/>
-      <c r="B170" s="26"/>
-      <c r="C170" s="50"/>
+      <c r="A170" s="50"/>
+      <c r="B170" s="50"/>
+      <c r="C170" s="28"/>
       <c r="D170" s="6" t="s">
         <v>245</v>
       </c>
@@ -8617,9 +8629,9 @@
       <c r="J170" s="15"/>
     </row>
     <row r="171" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A171" s="26"/>
-      <c r="B171" s="26"/>
-      <c r="C171" s="50"/>
+      <c r="A171" s="50"/>
+      <c r="B171" s="50"/>
+      <c r="C171" s="28"/>
       <c r="D171" s="6" t="s">
         <v>673</v>
       </c>
@@ -8639,9 +8651,9 @@
       <c r="J171" s="15"/>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A172" s="26"/>
-      <c r="B172" s="26"/>
-      <c r="C172" s="51"/>
+      <c r="A172" s="50"/>
+      <c r="B172" s="50"/>
+      <c r="C172" s="29"/>
       <c r="D172" s="6" t="s">
         <v>678</v>
       </c>
@@ -8661,13 +8673,13 @@
       <c r="J172" s="15"/>
     </row>
     <row r="173" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A173" s="25" t="s">
+      <c r="A173" s="54" t="s">
         <v>646</v>
       </c>
-      <c r="B173" s="25" t="s">
+      <c r="B173" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C173" s="38" t="s">
+      <c r="C173" s="30" t="s">
         <v>808</v>
       </c>
       <c r="D173" s="2" t="s">
@@ -8691,9 +8703,9 @@
       <c r="J173" s="16"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A174" s="25"/>
-      <c r="B174" s="25"/>
-      <c r="C174" s="40"/>
+      <c r="A174" s="54"/>
+      <c r="B174" s="54"/>
+      <c r="C174" s="31"/>
       <c r="D174" s="2" t="s">
         <v>247</v>
       </c>
@@ -8713,9 +8725,9 @@
       <c r="J174" s="16"/>
     </row>
     <row r="175" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A175" s="25"/>
-      <c r="B175" s="25"/>
-      <c r="C175" s="40"/>
+      <c r="A175" s="54"/>
+      <c r="B175" s="54"/>
+      <c r="C175" s="31"/>
       <c r="D175" s="2" t="s">
         <v>686</v>
       </c>
@@ -8735,9 +8747,9 @@
       <c r="J175" s="16"/>
     </row>
     <row r="176" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A176" s="25"/>
-      <c r="B176" s="25"/>
-      <c r="C176" s="39"/>
+      <c r="A176" s="54"/>
+      <c r="B176" s="54"/>
+      <c r="C176" s="32"/>
       <c r="D176" s="2" t="s">
         <v>248</v>
       </c>
@@ -8757,13 +8769,13 @@
       <c r="J176" s="16"/>
     </row>
     <row r="177" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="33" t="s">
         <v>424</v>
       </c>
-      <c r="B177" s="27" t="s">
+      <c r="B177" s="33" t="s">
         <v>425</v>
       </c>
-      <c r="C177" s="27" t="s">
+      <c r="C177" s="33" t="s">
         <v>809</v>
       </c>
       <c r="D177" s="3" t="s">
@@ -8787,9 +8799,9 @@
       <c r="J177" s="18"/>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A178" s="28"/>
-      <c r="B178" s="28"/>
-      <c r="C178" s="28"/>
+      <c r="A178" s="34"/>
+      <c r="B178" s="34"/>
+      <c r="C178" s="34"/>
       <c r="D178" s="3" t="s">
         <v>481</v>
       </c>
@@ -8809,9 +8821,9 @@
       <c r="J178" s="18"/>
     </row>
     <row r="179" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A179" s="28"/>
-      <c r="B179" s="28"/>
-      <c r="C179" s="28"/>
+      <c r="A179" s="34"/>
+      <c r="B179" s="34"/>
+      <c r="C179" s="34"/>
       <c r="D179" s="3" t="s">
         <v>482</v>
       </c>
@@ -8831,9 +8843,9 @@
       <c r="J179" s="18"/>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A180" s="28"/>
-      <c r="B180" s="28"/>
-      <c r="C180" s="28"/>
+      <c r="A180" s="34"/>
+      <c r="B180" s="34"/>
+      <c r="C180" s="34"/>
       <c r="D180" s="3" t="s">
         <v>433</v>
       </c>
@@ -8853,9 +8865,9 @@
       <c r="J180" s="18"/>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A181" s="28"/>
-      <c r="B181" s="28"/>
-      <c r="C181" s="28"/>
+      <c r="A181" s="34"/>
+      <c r="B181" s="34"/>
+      <c r="C181" s="34"/>
       <c r="D181" s="3" t="s">
         <v>434</v>
       </c>
@@ -8875,9 +8887,9 @@
       <c r="J181" s="18"/>
     </row>
     <row r="182" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A182" s="28"/>
-      <c r="B182" s="28"/>
-      <c r="C182" s="28"/>
+      <c r="A182" s="34"/>
+      <c r="B182" s="34"/>
+      <c r="C182" s="34"/>
       <c r="D182" s="3" t="s">
         <v>480</v>
       </c>
@@ -8897,9 +8909,9 @@
       <c r="J182" s="18"/>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A183" s="29"/>
-      <c r="B183" s="29"/>
-      <c r="C183" s="29"/>
+      <c r="A183" s="35"/>
+      <c r="B183" s="35"/>
+      <c r="C183" s="35"/>
       <c r="D183" s="3" t="s">
         <v>479</v>
       </c>
@@ -8919,13 +8931,13 @@
       <c r="J183" s="18"/>
     </row>
     <row r="184" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A184" s="30" t="s">
+      <c r="A184" s="46" t="s">
         <v>647</v>
       </c>
-      <c r="B184" s="30" t="s">
+      <c r="B184" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C184" s="30" t="s">
+      <c r="C184" s="46" t="s">
         <v>810</v>
       </c>
       <c r="D184" s="4" t="s">
@@ -8949,9 +8961,9 @@
       <c r="J184" s="14"/>
     </row>
     <row r="185" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A185" s="30"/>
-      <c r="B185" s="30"/>
-      <c r="C185" s="30"/>
+      <c r="A185" s="46"/>
+      <c r="B185" s="46"/>
+      <c r="C185" s="46"/>
       <c r="D185" s="4" t="s">
         <v>691</v>
       </c>
@@ -8973,9 +8985,9 @@
       <c r="J185" s="14"/>
     </row>
     <row r="186" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A186" s="30"/>
-      <c r="B186" s="30"/>
-      <c r="C186" s="30"/>
+      <c r="A186" s="46"/>
+      <c r="B186" s="46"/>
+      <c r="C186" s="46"/>
       <c r="D186" s="4" t="s">
         <v>649</v>
       </c>
@@ -8997,9 +9009,9 @@
       <c r="J186" s="14"/>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A187" s="30"/>
-      <c r="B187" s="30"/>
-      <c r="C187" s="30"/>
+      <c r="A187" s="46"/>
+      <c r="B187" s="46"/>
+      <c r="C187" s="46"/>
       <c r="D187" s="4" t="s">
         <v>650</v>
       </c>
@@ -9019,61 +9031,61 @@
       <c r="J187" s="14"/>
     </row>
     <row r="188" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A188" s="30"/>
-      <c r="B188" s="30"/>
-      <c r="C188" s="56" t="s">
+      <c r="A188" s="46"/>
+      <c r="B188" s="46"/>
+      <c r="C188" s="47" t="s">
         <v>766</v>
       </c>
-      <c r="D188" s="55" t="s">
+      <c r="D188" s="24" t="s">
         <v>700</v>
       </c>
-      <c r="E188" s="55" t="s">
+      <c r="E188" s="24" t="s">
         <v>694</v>
       </c>
-      <c r="F188" s="55" t="s">
+      <c r="F188" s="24" t="s">
         <v>695</v>
       </c>
-      <c r="G188" s="55" t="s">
+      <c r="G188" s="24" t="s">
         <v>693</v>
       </c>
-      <c r="H188" s="54">
+      <c r="H188" s="23">
         <v>3</v>
       </c>
-      <c r="I188" s="54" t="s">
-        <v>474</v>
-      </c>
-      <c r="J188" s="54"/>
+      <c r="I188" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="J188" s="23"/>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A189" s="30"/>
-      <c r="B189" s="30"/>
-      <c r="C189" s="57"/>
-      <c r="D189" s="55" t="s">
+      <c r="A189" s="46"/>
+      <c r="B189" s="46"/>
+      <c r="C189" s="48"/>
+      <c r="D189" s="24" t="s">
         <v>817</v>
       </c>
-      <c r="E189" s="55" t="s">
+      <c r="E189" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="F189" s="55" t="s">
+      <c r="F189" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="G189" s="55"/>
-      <c r="H189" s="54">
+      <c r="G189" s="24"/>
+      <c r="H189" s="23">
         <v>3</v>
       </c>
-      <c r="I189" s="54" t="s">
-        <v>474</v>
-      </c>
-      <c r="J189" s="54"/>
+      <c r="I189" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="J189" s="23"/>
     </row>
     <row r="190" spans="1:10" ht="231" x14ac:dyDescent="0.3">
-      <c r="A190" s="31" t="s">
+      <c r="A190" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B190" s="31" t="s">
+      <c r="B190" s="52" t="s">
         <v>392</v>
       </c>
-      <c r="C190" s="35" t="s">
+      <c r="C190" s="43" t="s">
         <v>812</v>
       </c>
       <c r="D190" s="5" t="s">
@@ -9097,9 +9109,9 @@
       <c r="J190" s="17"/>
     </row>
     <row r="191" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A191" s="31"/>
-      <c r="B191" s="31"/>
-      <c r="C191" s="36"/>
+      <c r="A191" s="52"/>
+      <c r="B191" s="52"/>
+      <c r="C191" s="44"/>
       <c r="D191" s="5" t="s">
         <v>81</v>
       </c>
@@ -9119,9 +9131,9 @@
       <c r="J191" s="17"/>
     </row>
     <row r="192" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A192" s="31"/>
-      <c r="B192" s="31"/>
-      <c r="C192" s="36"/>
+      <c r="A192" s="52"/>
+      <c r="B192" s="52"/>
+      <c r="C192" s="44"/>
       <c r="D192" s="5" t="s">
         <v>370</v>
       </c>
@@ -9143,9 +9155,9 @@
       <c r="J192" s="17"/>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A193" s="31"/>
-      <c r="B193" s="31"/>
-      <c r="C193" s="36"/>
+      <c r="A193" s="52"/>
+      <c r="B193" s="52"/>
+      <c r="C193" s="44"/>
       <c r="D193" s="5" t="s">
         <v>82</v>
       </c>
@@ -9165,9 +9177,9 @@
       <c r="J193" s="17"/>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A194" s="31"/>
-      <c r="B194" s="31"/>
-      <c r="C194" s="37"/>
+      <c r="A194" s="52"/>
+      <c r="B194" s="52"/>
+      <c r="C194" s="45"/>
       <c r="D194" s="5" t="s">
         <v>716</v>
       </c>
@@ -9187,61 +9199,61 @@
       <c r="J194" s="17"/>
     </row>
     <row r="195" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A195" s="31"/>
-      <c r="B195" s="31"/>
-      <c r="C195" s="45" t="s">
+      <c r="A195" s="52"/>
+      <c r="B195" s="52"/>
+      <c r="C195" s="41" t="s">
         <v>766</v>
       </c>
-      <c r="D195" s="46" t="s">
+      <c r="D195" s="21" t="s">
         <v>393</v>
       </c>
-      <c r="E195" s="46" t="s">
+      <c r="E195" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="F195" s="46" t="s">
+      <c r="F195" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="G195" s="46" t="s">
+      <c r="G195" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="H195" s="47">
+      <c r="H195" s="22">
         <v>3</v>
       </c>
-      <c r="I195" s="47" t="s">
+      <c r="I195" s="22" t="s">
         <v>472</v>
       </c>
-      <c r="J195" s="47"/>
+      <c r="J195" s="22"/>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A196" s="31"/>
-      <c r="B196" s="31"/>
-      <c r="C196" s="48"/>
-      <c r="D196" s="46" t="s">
+      <c r="A196" s="52"/>
+      <c r="B196" s="52"/>
+      <c r="C196" s="42"/>
+      <c r="D196" s="21" t="s">
         <v>398</v>
       </c>
-      <c r="E196" s="46" t="s">
+      <c r="E196" s="21" t="s">
         <v>813</v>
       </c>
-      <c r="F196" s="46" t="s">
+      <c r="F196" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="G196" s="46"/>
-      <c r="H196" s="47">
+      <c r="G196" s="21"/>
+      <c r="H196" s="22">
         <v>3</v>
       </c>
-      <c r="I196" s="47" t="s">
+      <c r="I196" s="22" t="s">
         <v>472</v>
       </c>
-      <c r="J196" s="47"/>
+      <c r="J196" s="22"/>
     </row>
     <row r="197" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A197" s="26" t="s">
+      <c r="A197" s="50" t="s">
         <v>377</v>
       </c>
-      <c r="B197" s="26" t="s">
+      <c r="B197" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C197" s="49" t="s">
+      <c r="C197" s="27" t="s">
         <v>814</v>
       </c>
       <c r="D197" s="6" t="s">
@@ -9265,9 +9277,9 @@
       <c r="J197" s="15"/>
     </row>
     <row r="198" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A198" s="26"/>
-      <c r="B198" s="26"/>
-      <c r="C198" s="50"/>
+      <c r="A198" s="50"/>
+      <c r="B198" s="50"/>
+      <c r="C198" s="28"/>
       <c r="D198" s="6" t="s">
         <v>84</v>
       </c>
@@ -9289,9 +9301,9 @@
       <c r="J198" s="15"/>
     </row>
     <row r="199" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A199" s="26"/>
-      <c r="B199" s="26"/>
-      <c r="C199" s="50"/>
+      <c r="A199" s="50"/>
+      <c r="B199" s="50"/>
+      <c r="C199" s="28"/>
       <c r="D199" s="6" t="s">
         <v>378</v>
       </c>
@@ -9311,9 +9323,9 @@
       <c r="J199" s="15"/>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A200" s="26"/>
-      <c r="B200" s="26"/>
-      <c r="C200" s="50"/>
+      <c r="A200" s="50"/>
+      <c r="B200" s="50"/>
+      <c r="C200" s="28"/>
       <c r="D200" s="6" t="s">
         <v>85</v>
       </c>
@@ -9333,9 +9345,9 @@
       <c r="J200" s="15"/>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A201" s="26"/>
-      <c r="B201" s="26"/>
-      <c r="C201" s="51"/>
+      <c r="A201" s="50"/>
+      <c r="B201" s="50"/>
+      <c r="C201" s="29"/>
       <c r="D201" s="6" t="s">
         <v>379</v>
       </c>
@@ -9355,13 +9367,13 @@
       <c r="J201" s="15"/>
     </row>
     <row r="202" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A202" s="25" t="s">
+      <c r="A202" s="54" t="s">
         <v>389</v>
       </c>
-      <c r="B202" s="25" t="s">
+      <c r="B202" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="C202" s="38" t="s">
+      <c r="C202" s="30" t="s">
         <v>815</v>
       </c>
       <c r="D202" s="2" t="s">
@@ -9385,9 +9397,9 @@
       <c r="J202" s="16"/>
     </row>
     <row r="203" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A203" s="25"/>
-      <c r="B203" s="25"/>
-      <c r="C203" s="40"/>
+      <c r="A203" s="54"/>
+      <c r="B203" s="54"/>
+      <c r="C203" s="31"/>
       <c r="D203" s="2" t="s">
         <v>99</v>
       </c>
@@ -9409,9 +9421,9 @@
       <c r="J203" s="16"/>
     </row>
     <row r="204" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A204" s="25"/>
-      <c r="B204" s="25"/>
-      <c r="C204" s="40"/>
+      <c r="A204" s="54"/>
+      <c r="B204" s="54"/>
+      <c r="C204" s="31"/>
       <c r="D204" s="2" t="s">
         <v>390</v>
       </c>
@@ -9431,9 +9443,9 @@
       <c r="J204" s="16"/>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A205" s="25"/>
-      <c r="B205" s="25"/>
-      <c r="C205" s="40"/>
+      <c r="A205" s="54"/>
+      <c r="B205" s="54"/>
+      <c r="C205" s="31"/>
       <c r="D205" s="2" t="s">
         <v>100</v>
       </c>
@@ -9453,9 +9465,9 @@
       <c r="J205" s="16"/>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A206" s="25"/>
-      <c r="B206" s="25"/>
-      <c r="C206" s="39"/>
+      <c r="A206" s="54"/>
+      <c r="B206" s="54"/>
+      <c r="C206" s="32"/>
       <c r="D206" s="2" t="s">
         <v>391</v>
       </c>
@@ -9475,13 +9487,13 @@
       <c r="J206" s="16"/>
     </row>
     <row r="207" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A207" s="24" t="s">
+      <c r="A207" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="B207" s="24" t="s">
+      <c r="B207" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C207" s="27" t="s">
+      <c r="C207" s="33" t="s">
         <v>816</v>
       </c>
       <c r="D207" s="3" t="s">
@@ -9505,9 +9517,9 @@
       <c r="J207" s="18"/>
     </row>
     <row r="208" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A208" s="24"/>
-      <c r="B208" s="24"/>
-      <c r="C208" s="28"/>
+      <c r="A208" s="55"/>
+      <c r="B208" s="55"/>
+      <c r="C208" s="34"/>
       <c r="D208" s="3" t="s">
         <v>94</v>
       </c>
@@ -9527,9 +9539,9 @@
       <c r="J208" s="18"/>
     </row>
     <row r="209" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A209" s="24"/>
-      <c r="B209" s="24"/>
-      <c r="C209" s="28"/>
+      <c r="A209" s="55"/>
+      <c r="B209" s="55"/>
+      <c r="C209" s="34"/>
       <c r="D209" s="3" t="s">
         <v>419</v>
       </c>
@@ -9549,9 +9561,9 @@
       <c r="J209" s="18"/>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A210" s="24"/>
-      <c r="B210" s="24"/>
-      <c r="C210" s="28"/>
+      <c r="A210" s="55"/>
+      <c r="B210" s="55"/>
+      <c r="C210" s="34"/>
       <c r="D210" s="3" t="s">
         <v>95</v>
       </c>
@@ -9571,9 +9583,9 @@
       <c r="J210" s="18"/>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A211" s="24"/>
-      <c r="B211" s="24"/>
-      <c r="C211" s="29"/>
+      <c r="A211" s="55"/>
+      <c r="B211" s="55"/>
+      <c r="C211" s="35"/>
       <c r="D211" s="3" t="s">
         <v>711</v>
       </c>
@@ -9593,13 +9605,13 @@
       <c r="J211" s="18"/>
     </row>
     <row r="212" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A212" s="30" t="s">
+      <c r="A212" s="46" t="s">
         <v>827</v>
       </c>
-      <c r="B212" s="30" t="s">
+      <c r="B212" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="C212" s="32" t="s">
+      <c r="C212" s="38" t="s">
         <v>811</v>
       </c>
       <c r="D212" s="4" t="s">
@@ -9623,9 +9635,9 @@
       <c r="J212" s="14"/>
     </row>
     <row r="213" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A213" s="30"/>
-      <c r="B213" s="30"/>
-      <c r="C213" s="33"/>
+      <c r="A213" s="46"/>
+      <c r="B213" s="46"/>
+      <c r="C213" s="39"/>
       <c r="D213" s="4" t="s">
         <v>830</v>
       </c>
@@ -9645,9 +9657,9 @@
       <c r="J213" s="14"/>
     </row>
     <row r="214" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A214" s="30"/>
-      <c r="B214" s="30"/>
-      <c r="C214" s="33"/>
+      <c r="A214" s="46"/>
+      <c r="B214" s="46"/>
+      <c r="C214" s="39"/>
       <c r="D214" s="4" t="s">
         <v>831</v>
       </c>
@@ -9667,9 +9679,9 @@
       <c r="J214" s="14"/>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A215" s="30"/>
-      <c r="B215" s="30"/>
-      <c r="C215" s="34"/>
+      <c r="A215" s="46"/>
+      <c r="B215" s="46"/>
+      <c r="C215" s="40"/>
       <c r="D215" s="4" t="s">
         <v>832</v>
       </c>
@@ -9689,13 +9701,13 @@
       <c r="J215" s="14"/>
     </row>
     <row r="216" spans="1:10" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A216" s="31" t="s">
+      <c r="A216" s="52" t="s">
         <v>828</v>
       </c>
-      <c r="B216" s="31" t="s">
+      <c r="B216" s="52" t="s">
         <v>820</v>
       </c>
-      <c r="C216" s="35" t="s">
+      <c r="C216" s="43" t="s">
         <v>821</v>
       </c>
       <c r="D216" s="5" t="s">
@@ -9719,9 +9731,9 @@
       <c r="J216" s="17"/>
     </row>
     <row r="217" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A217" s="31"/>
-      <c r="B217" s="31"/>
-      <c r="C217" s="36"/>
+      <c r="A217" s="52"/>
+      <c r="B217" s="52"/>
+      <c r="C217" s="44"/>
       <c r="D217" s="5" t="s">
         <v>834</v>
       </c>
@@ -9743,9 +9755,9 @@
       <c r="J217" s="17"/>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A218" s="31"/>
-      <c r="B218" s="31"/>
-      <c r="C218" s="36"/>
+      <c r="A218" s="52"/>
+      <c r="B218" s="52"/>
+      <c r="C218" s="44"/>
       <c r="D218" s="5" t="s">
         <v>835</v>
       </c>
@@ -9765,9 +9777,9 @@
       <c r="J218" s="17"/>
     </row>
     <row r="219" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A219" s="31"/>
-      <c r="B219" s="31"/>
-      <c r="C219" s="36"/>
+      <c r="A219" s="52"/>
+      <c r="B219" s="52"/>
+      <c r="C219" s="44"/>
       <c r="D219" s="5" t="s">
         <v>836</v>
       </c>
@@ -9787,9 +9799,9 @@
       <c r="J219" s="17"/>
     </row>
     <row r="220" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A220" s="31"/>
-      <c r="B220" s="31"/>
-      <c r="C220" s="37"/>
+      <c r="A220" s="52"/>
+      <c r="B220" s="52"/>
+      <c r="C220" s="45"/>
       <c r="D220" s="5" t="s">
         <v>837</v>
       </c>
@@ -9811,6 +9823,116 @@
   </sheetData>
   <autoFilter ref="A1:J220"/>
   <mergeCells count="134">
+    <mergeCell ref="A202:A206"/>
+    <mergeCell ref="B202:B206"/>
+    <mergeCell ref="A207:A211"/>
+    <mergeCell ref="B207:B211"/>
+    <mergeCell ref="B212:B215"/>
+    <mergeCell ref="A190:A196"/>
+    <mergeCell ref="B190:B196"/>
+    <mergeCell ref="A197:A201"/>
+    <mergeCell ref="B197:B201"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="B2:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B37:B44"/>
+    <mergeCell ref="A184:A189"/>
+    <mergeCell ref="B184:B189"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="A52:A58"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="A149:A155"/>
+    <mergeCell ref="B142:B148"/>
+    <mergeCell ref="B149:B155"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="B111:B115"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="A105:A110"/>
+    <mergeCell ref="B105:B110"/>
+    <mergeCell ref="A128:A132"/>
+    <mergeCell ref="B128:B132"/>
+    <mergeCell ref="A156:A162"/>
+    <mergeCell ref="A167:A172"/>
+    <mergeCell ref="B167:B172"/>
+    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="B21:B28"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A81:A85"/>
+    <mergeCell ref="A216:A220"/>
+    <mergeCell ref="B216:B220"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="A173:A176"/>
+    <mergeCell ref="B173:B176"/>
+    <mergeCell ref="A177:A183"/>
+    <mergeCell ref="B177:B183"/>
+    <mergeCell ref="A142:A148"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="B124:B127"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="B81:B85"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:B75"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="A133:A136"/>
+    <mergeCell ref="B133:B136"/>
+    <mergeCell ref="A163:A166"/>
+    <mergeCell ref="B163:B166"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="A86:A90"/>
+    <mergeCell ref="B86:B90"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A93:A96"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="B156:B162"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="C69:C75"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="C81:C85"/>
+    <mergeCell ref="C216:C220"/>
+    <mergeCell ref="C37:C44"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C105:C109"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="J103:J104"/>
+    <mergeCell ref="C103:C104"/>
     <mergeCell ref="C197:C201"/>
     <mergeCell ref="C202:C206"/>
     <mergeCell ref="C207:C211"/>
@@ -9835,116 +9957,6 @@
     <mergeCell ref="C133:C136"/>
     <mergeCell ref="C137:C141"/>
     <mergeCell ref="C97:C102"/>
-    <mergeCell ref="C105:C109"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="J103:J104"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="C69:C75"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="C81:C85"/>
-    <mergeCell ref="C216:C220"/>
-    <mergeCell ref="C37:C44"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B81:B85"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:B75"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="A133:A136"/>
-    <mergeCell ref="B133:B136"/>
-    <mergeCell ref="A163:A166"/>
-    <mergeCell ref="B163:B166"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="B97:B102"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="B86:B90"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="B21:B28"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A216:A220"/>
-    <mergeCell ref="B216:B220"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="B2:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B37:B44"/>
-    <mergeCell ref="A184:A189"/>
-    <mergeCell ref="B184:B189"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="A52:A58"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="A149:A155"/>
-    <mergeCell ref="B142:B148"/>
-    <mergeCell ref="B149:B155"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="B111:B115"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="A105:A110"/>
-    <mergeCell ref="B105:B110"/>
-    <mergeCell ref="A128:A132"/>
-    <mergeCell ref="B128:B132"/>
-    <mergeCell ref="A156:A162"/>
-    <mergeCell ref="A167:A172"/>
-    <mergeCell ref="B167:B172"/>
-    <mergeCell ref="A173:A176"/>
-    <mergeCell ref="B173:B176"/>
-    <mergeCell ref="A177:A183"/>
-    <mergeCell ref="B177:B183"/>
-    <mergeCell ref="A142:A148"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="B124:B127"/>
-    <mergeCell ref="A119:A123"/>
-    <mergeCell ref="B119:B123"/>
-    <mergeCell ref="B156:B162"/>
-    <mergeCell ref="A137:A141"/>
-    <mergeCell ref="B137:B141"/>
-    <mergeCell ref="A202:A206"/>
-    <mergeCell ref="B202:B206"/>
-    <mergeCell ref="A207:A211"/>
-    <mergeCell ref="B207:B211"/>
-    <mergeCell ref="B212:B215"/>
-    <mergeCell ref="A190:A196"/>
-    <mergeCell ref="B190:B196"/>
-    <mergeCell ref="A197:A201"/>
-    <mergeCell ref="B197:B201"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9974,10 +9986,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="57" t="s">
         <v>424</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="57" t="s">
         <v>425</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -10001,8 +10013,8 @@
       <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="10" t="s">
         <v>481</v>
       </c>
@@ -10022,8 +10034,8 @@
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="10" t="s">
         <v>482</v>
       </c>
@@ -10043,8 +10055,8 @@
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="10" t="s">
         <v>433</v>
       </c>
@@ -10064,8 +10076,8 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="10" t="s">
         <v>434</v>
       </c>
@@ -10085,8 +10097,8 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>480</v>
       </c>
@@ -10106,8 +10118,8 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="10" t="s">
         <v>479</v>
       </c>
@@ -10127,10 +10139,10 @@
       <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="198" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="60" t="s">
         <v>647</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="60" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -10154,8 +10166,8 @@
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="10" t="s">
         <v>691</v>
       </c>
@@ -10177,8 +10189,8 @@
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="10" t="s">
         <v>649</v>
       </c>
@@ -10200,8 +10212,8 @@
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="10" t="s">
         <v>700</v>
       </c>
@@ -10223,8 +10235,8 @@
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="10" t="s">
         <v>650</v>
       </c>
@@ -10244,10 +10256,10 @@
       <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" ht="132" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="57" t="s">
         <v>343</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -10271,8 +10283,8 @@
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="10" t="s">
         <v>68</v>
       </c>
@@ -10292,8 +10304,8 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="10" t="s">
         <v>69</v>
       </c>
@@ -10313,8 +10325,8 @@
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="10" t="s">
         <v>710</v>
       </c>
@@ -10334,10 +10346,10 @@
       <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" ht="231" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="57" t="s">
         <v>392</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -10361,8 +10373,8 @@
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="10" t="s">
         <v>81</v>
       </c>
@@ -10384,8 +10396,8 @@
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="10" t="s">
         <v>370</v>
       </c>
@@ -10405,8 +10417,8 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="10" t="s">
         <v>393</v>
       </c>
@@ -10426,8 +10438,8 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="10" t="s">
         <v>398</v>
       </c>
@@ -10449,8 +10461,8 @@
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="10" t="s">
         <v>82</v>
       </c>
@@ -10470,8 +10482,8 @@
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="10" t="s">
         <v>716</v>
       </c>
@@ -10491,10 +10503,10 @@
       <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="61" t="s">
         <v>377</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="61" t="s">
         <v>75</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -10518,8 +10530,8 @@
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="8" t="s">
         <v>84</v>
       </c>
@@ -10541,8 +10553,8 @@
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="8" t="s">
         <v>378</v>
       </c>
@@ -10562,8 +10574,8 @@
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="8" t="s">
         <v>85</v>
       </c>
@@ -10583,8 +10595,8 @@
       <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="8" t="s">
         <v>379</v>
       </c>
@@ -10604,10 +10616,10 @@
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.3">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="60" t="s">
         <v>389</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="60" t="s">
         <v>79</v>
       </c>
       <c r="C29" s="10" t="s">
@@ -10631,8 +10643,8 @@
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="10" t="s">
         <v>99</v>
       </c>
@@ -10654,8 +10666,8 @@
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="10" t="s">
         <v>390</v>
       </c>
@@ -10675,8 +10687,8 @@
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="10" t="s">
         <v>100</v>
       </c>
@@ -10696,8 +10708,8 @@
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="60"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="10" t="s">
         <v>391</v>
       </c>
@@ -10717,10 +10729,10 @@
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="57" t="s">
         <v>92</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -10744,8 +10756,8 @@
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="10" t="s">
         <v>94</v>
       </c>
@@ -10765,8 +10777,8 @@
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
       <c r="C36" s="10" t="s">
         <v>419</v>
       </c>
@@ -10786,8 +10798,8 @@
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="10" t="s">
         <v>95</v>
       </c>
@@ -10807,8 +10819,8 @@
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="59"/>
+      <c r="B38" s="59"/>
       <c r="C38" s="10" t="s">
         <v>711</v>
       </c>

</xml_diff>